<commit_message>
avg profile of agestruct
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/soc-conflicts analysis.xlsx
+++ b/migforecasting/social conflicts/soc-conflicts analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="conflicts" sheetId="1" r:id="rId1"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,67 +808,67 @@
         <v>24</v>
       </c>
       <c r="F9" s="5">
-        <f>AVERAGE(F5:F7)</f>
+        <f t="shared" ref="F9:U9" si="0">AVERAGE(F5:F7)</f>
         <v>58716.999999999993</v>
       </c>
       <c r="G9" s="5">
-        <f>AVERAGE(G5:G7)</f>
+        <f t="shared" si="0"/>
         <v>0.18681564335698408</v>
       </c>
       <c r="H9" s="5">
-        <f>AVERAGE(H5:H7)</f>
+        <f t="shared" si="0"/>
         <v>26901.343810000002</v>
       </c>
       <c r="I9" s="5">
-        <f>AVERAGE(I5:I7)</f>
+        <f t="shared" si="0"/>
         <v>0.91388570390790225</v>
       </c>
       <c r="J9" s="5">
-        <f>AVERAGE(J5:J7)</f>
+        <f t="shared" si="0"/>
         <v>3.6417490580994437E-2</v>
       </c>
       <c r="K9" s="5">
-        <f>AVERAGE(K5:K7)</f>
+        <f t="shared" si="0"/>
         <v>49.960971683666081</v>
       </c>
       <c r="L9" s="5">
-        <f>AVERAGE(L5:L7)</f>
+        <f t="shared" si="0"/>
         <v>36.516666666666673</v>
       </c>
       <c r="M9" s="5">
-        <f>AVERAGE(M5:M7)</f>
+        <f t="shared" si="0"/>
         <v>3.6379309114502635E-3</v>
       </c>
       <c r="N9" s="5">
-        <f>AVERAGE(N5:N7)</f>
+        <f t="shared" si="0"/>
         <v>3.2938233580593473E-3</v>
       </c>
       <c r="O9" s="5">
-        <f>AVERAGE(O5:O7)</f>
+        <f t="shared" si="0"/>
         <v>1.4024513522607722E-2</v>
       </c>
       <c r="P9" s="5">
-        <f>AVERAGE(P5:P7)</f>
+        <f t="shared" si="0"/>
         <v>1.8506174289879558</v>
       </c>
       <c r="Q9" s="5">
-        <f>AVERAGE(Q5:Q7)</f>
+        <f t="shared" si="0"/>
         <v>1.1688063906689699</v>
       </c>
       <c r="R9" s="5">
-        <f>AVERAGE(R5:R7)</f>
+        <f t="shared" si="0"/>
         <v>33.901507691368209</v>
       </c>
       <c r="S9" s="5">
-        <f>AVERAGE(S5:S7)</f>
+        <f t="shared" si="0"/>
         <v>9.0806833662219219E-4</v>
       </c>
       <c r="T9" s="5">
-        <f>AVERAGE(T5:T7)</f>
+        <f t="shared" si="0"/>
         <v>6.3673122480590635E-2</v>
       </c>
       <c r="U9" s="5">
-        <f>AVERAGE(U5:U7)</f>
+        <f t="shared" si="0"/>
         <v>138.31016875922501</v>
       </c>
     </row>
@@ -1356,51 +1356,51 @@
         <v>5.8196666666666667E-2</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" ref="G25:S25" si="0">AVERAGE(G14,G17,G20)</f>
+        <f t="shared" ref="G25:R25" si="1">AVERAGE(G14,G17,G20)</f>
         <v>7.1566666666666667E-2</v>
       </c>
       <c r="H25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6796666666666671E-2</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1953333333333331E-2</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.2540000000000001E-2</v>
       </c>
       <c r="K25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0973333333333334E-2</v>
       </c>
       <c r="L25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2136666666666673E-2</v>
       </c>
       <c r="M25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4543333333333336E-2</v>
       </c>
       <c r="N25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.535E-2</v>
       </c>
       <c r="O25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9646666666666662E-2</v>
       </c>
       <c r="P25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13522000000000001</v>
       </c>
       <c r="Q25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.1633333333333336E-2</v>
       </c>
       <c r="R25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1553333333333334E-2</v>
       </c>
       <c r="S25" s="7">
@@ -1420,55 +1420,55 @@
         <v>6.5433333333333329E-2</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" ref="G26:S26" si="1">AVERAGE(G15,G18,G21)</f>
+        <f t="shared" ref="G26:S26" si="2">AVERAGE(G15,G18,G21)</f>
         <v>8.0166666666666664E-2</v>
       </c>
       <c r="H26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3579999999999993E-2</v>
       </c>
       <c r="I26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.7373333333333332E-2</v>
       </c>
       <c r="J26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6416666666666662E-2</v>
       </c>
       <c r="K26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1016666666666662E-2</v>
       </c>
       <c r="L26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3390000000000011E-2</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1316666666666676E-2</v>
       </c>
       <c r="N26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.5023333333333331E-2</v>
       </c>
       <c r="O26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0103333333333337E-2</v>
       </c>
       <c r="P26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12418666666666667</v>
       </c>
       <c r="Q26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3910000000000003E-2</v>
       </c>
       <c r="R26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.277666666666667E-2</v>
       </c>
       <c r="S26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5296666666666661E-2</v>
       </c>
     </row>
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:V34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,18 +2747,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:I9">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K9">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:L9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -2770,55 +2770,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L9">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M9">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N9">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5:O9">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P5:P9">
+  <conditionalFormatting sqref="Q5:Q9">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -2830,7 +2782,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5:Q9">
+  <conditionalFormatting sqref="R5:R9">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -2842,7 +2794,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R9">
+  <conditionalFormatting sqref="S5:S9">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -2854,31 +2806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5:S9">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T5:T9">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U5:U9">
+  <conditionalFormatting sqref="V5:V9">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -2890,19 +2818,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V9">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H9">
+  <conditionalFormatting sqref="I12:I13 I15:I16">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -2914,7 +2830,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I13 I15:I16">
+  <conditionalFormatting sqref="M12:M13 M15:M16">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2926,7 +2842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M12:M13 M15:M16">
+  <conditionalFormatting sqref="H12:H13 H15:H16">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2938,7 +2854,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H13 H15:H16">
+  <conditionalFormatting sqref="J12:J13 J15:J16">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2950,7 +2866,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J13 J15:J16">
+  <conditionalFormatting sqref="K12:K13 K15:K16">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2962,7 +2878,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12:K13 K15:K16">
+  <conditionalFormatting sqref="L12:L13 L15:L16">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2974,7 +2890,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L12:L13 L15:L16">
+  <conditionalFormatting sqref="N12:N13 N15:N16">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2986,7 +2902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12:N13 N15:N16">
+  <conditionalFormatting sqref="O12:O13 O15:O16">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2998,7 +2914,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O12:O13 O15:O16">
+  <conditionalFormatting sqref="P12:P13 P15:P16">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3010,7 +2926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P12:P13 P15:P16">
+  <conditionalFormatting sqref="Q12:Q13 Q15:Q16">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3022,7 +2938,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q12:Q13 Q15:Q16">
+  <conditionalFormatting sqref="R12:R13 R15:R16">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3034,7 +2950,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R12:R13 R15:R16">
+  <conditionalFormatting sqref="S12:S13 S15:S16">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3046,7 +2962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12:S13 S15:S16">
+  <conditionalFormatting sqref="U12:U13 U15:U16">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3058,7 +2974,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U12:U13 U15:U16">
+  <conditionalFormatting sqref="V12:V13 V15:V16">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3070,7 +2986,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V12:V13 V15:V16">
+  <conditionalFormatting sqref="I20:I22">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3082,19 +2998,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I22">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H22">
+  <conditionalFormatting sqref="I18:I22">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3106,7 +3010,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I22">
+  <conditionalFormatting sqref="V18:V22">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3118,7 +3022,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V18:V22">
+  <conditionalFormatting sqref="S18:S22">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3130,7 +3034,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18:S22">
+  <conditionalFormatting sqref="R18:R22">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3142,7 +3046,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R18:R22">
+  <conditionalFormatting sqref="L18:L22">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3154,7 +3058,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18:L22">
+  <conditionalFormatting sqref="Q18:Q22">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3166,19 +3070,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18:Q22">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J9">
+  <conditionalFormatting sqref="I30:I34">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3190,7 +3082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:I34">
+  <conditionalFormatting sqref="L30:L34">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3202,7 +3094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30:L34">
+  <conditionalFormatting sqref="V30:V34">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3214,7 +3106,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V30:V34">
+  <conditionalFormatting sqref="Q30:Q34">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3226,7 +3118,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q30:Q34">
+  <conditionalFormatting sqref="R30:R34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3238,20 +3130,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R30:R34">
+  <conditionalFormatting sqref="S30:S34">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30:S34">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
data on Laishevsky mun. dist. (against highway)
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/soc-conflicts analysis.xlsx
+++ b/migforecasting/social conflicts/soc-conflicts analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="anti-garbage" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="72">
   <si>
     <t>saldo</t>
   </si>
@@ -234,6 +234,12 @@
   <si>
     <t>Котлас</t>
   </si>
+  <si>
+    <t>анти-индустриальный</t>
+  </si>
+  <si>
+    <t>Лаишевский МР</t>
+  </si>
 </sst>
 </file>
 
@@ -243,12 +249,20 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -343,18 +357,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -366,35 +380,35 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -409,6 +423,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2210,59 +2228,59 @@
         <v>41</v>
       </c>
       <c r="F30" s="7">
-        <f>AVERAGE(F16,F18,F20,F22,F24)</f>
+        <f t="shared" ref="F30:S30" si="3">AVERAGE(F16,F18,F20,F22,F24)</f>
         <v>4.8851999999999993E-2</v>
       </c>
       <c r="G30" s="7">
-        <f>AVERAGE(G16,G18,G20,G22,G24)</f>
+        <f t="shared" si="3"/>
         <v>6.6384000000000012E-2</v>
       </c>
       <c r="H30" s="7">
-        <f>AVERAGE(H16,H18,H20,H22,H24)</f>
+        <f t="shared" si="3"/>
         <v>6.3287999999999997E-2</v>
       </c>
       <c r="I30" s="7">
-        <f>AVERAGE(I16,I18,I20,I22,I24)</f>
+        <f t="shared" si="3"/>
         <v>5.1112000000000005E-2</v>
       </c>
       <c r="J30" s="7">
-        <f>AVERAGE(J16,J18,J20,J22,J24)</f>
+        <f t="shared" si="3"/>
         <v>4.2570000000000004E-2</v>
       </c>
       <c r="K30" s="7">
-        <f>AVERAGE(K16,K18,K20,K22,K24)</f>
+        <f t="shared" si="3"/>
         <v>3.6932E-2</v>
       </c>
       <c r="L30" s="7">
-        <f>AVERAGE(L16,L18,L20,L22,L24)</f>
+        <f t="shared" si="3"/>
         <v>5.9919999999999994E-2</v>
       </c>
       <c r="M30" s="7">
-        <f>AVERAGE(M16,M18,M20,M22,M24)</f>
+        <f t="shared" si="3"/>
         <v>7.7354000000000006E-2</v>
       </c>
       <c r="N30" s="7">
-        <f>AVERAGE(N16,N18,N20,N22,N24)</f>
+        <f t="shared" si="3"/>
         <v>7.6800000000000007E-2</v>
       </c>
       <c r="O30" s="7">
-        <f>AVERAGE(O16,O18,O20,O22,O24)</f>
+        <f t="shared" si="3"/>
         <v>7.0716000000000001E-2</v>
       </c>
       <c r="P30" s="7">
-        <f>AVERAGE(P16,P18,P20,P22,P24)</f>
+        <f t="shared" si="3"/>
         <v>0.13745000000000002</v>
       </c>
       <c r="Q30" s="7">
-        <f>AVERAGE(Q16,Q18,Q20,Q22,Q24)</f>
+        <f t="shared" si="3"/>
         <v>8.2867999999999997E-2</v>
       </c>
       <c r="R30" s="7">
-        <f>AVERAGE(R16,R18,R20,R22,R24)</f>
+        <f t="shared" si="3"/>
         <v>0.10084</v>
       </c>
       <c r="S30" s="7">
-        <f>AVERAGE(S16,S18,S20,S22,S24)</f>
+        <f t="shared" si="3"/>
         <v>8.4920000000000009E-2</v>
       </c>
     </row>
@@ -2277,59 +2295,59 @@
         <v>42</v>
       </c>
       <c r="F31" s="7">
-        <f>AVERAGE(F17,F19,F21,F23,F25)</f>
+        <f t="shared" ref="F31:S31" si="4">AVERAGE(F17,F19,F21,F23,F25)</f>
         <v>5.5567999999999992E-2</v>
       </c>
       <c r="G31" s="7">
-        <f>AVERAGE(G17,G19,G21,G23,G25)</f>
+        <f t="shared" si="4"/>
         <v>7.4520000000000003E-2</v>
       </c>
       <c r="H31" s="7">
-        <f>AVERAGE(H17,H19,H21,H23,H25)</f>
+        <f t="shared" si="4"/>
         <v>7.077399999999999E-2</v>
       </c>
       <c r="I31" s="7">
-        <f>AVERAGE(I17,I19,I21,I23,I25)</f>
+        <f t="shared" si="4"/>
         <v>5.7190000000000005E-2</v>
       </c>
       <c r="J31" s="7">
-        <f>AVERAGE(J17,J19,J21,J23,J25)</f>
+        <f t="shared" si="4"/>
         <v>4.7094000000000004E-2</v>
       </c>
       <c r="K31" s="7">
-        <f>AVERAGE(K17,K19,K21,K23,K25)</f>
+        <f t="shared" si="4"/>
         <v>4.8735999999999995E-2</v>
       </c>
       <c r="L31" s="7">
-        <f>AVERAGE(L17,L19,L21,L23,L25)</f>
+        <f t="shared" si="4"/>
         <v>7.2798000000000002E-2</v>
       </c>
       <c r="M31" s="7">
-        <f>AVERAGE(M17,M19,M21,M23,M25)</f>
+        <f t="shared" si="4"/>
         <v>8.3370000000000014E-2</v>
       </c>
       <c r="N31" s="7">
-        <f>AVERAGE(N17,N19,N21,N23,N25)</f>
+        <f t="shared" si="4"/>
         <v>7.7202000000000007E-2</v>
       </c>
       <c r="O31" s="7">
-        <f>AVERAGE(O17,O19,O21,O23,O25)</f>
+        <f t="shared" si="4"/>
         <v>7.1142000000000011E-2</v>
       </c>
       <c r="P31" s="7">
-        <f>AVERAGE(P17,P19,P21,P23,P25)</f>
+        <f t="shared" si="4"/>
         <v>0.125668</v>
       </c>
       <c r="Q31" s="7">
-        <f>AVERAGE(Q17,Q19,Q21,Q23,Q25)</f>
+        <f t="shared" si="4"/>
         <v>7.4862000000000012E-2</v>
       </c>
       <c r="R31" s="7">
-        <f>AVERAGE(R17,R19,R21,R23,R25)</f>
+        <f t="shared" si="4"/>
         <v>7.9177999999999998E-2</v>
       </c>
       <c r="S31" s="7">
-        <f>AVERAGE(S17,S19,S21,S23,S25)</f>
+        <f t="shared" si="4"/>
         <v>6.1881999999999993E-2</v>
       </c>
     </row>
@@ -2528,7 +2546,7 @@
         <v>21</v>
       </c>
       <c r="D38" s="9">
-        <f t="shared" ref="D38:D40" si="3">D37+1</f>
+        <f t="shared" ref="D38:D40" si="5">D37+1</f>
         <v>2020</v>
       </c>
       <c r="E38" s="1">
@@ -2591,7 +2609,7 @@
         <v>21</v>
       </c>
       <c r="D39" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="E39" s="1">
@@ -2652,7 +2670,7 @@
         <v>21</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2022</v>
       </c>
       <c r="E40" s="1">
@@ -8042,18 +8060,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:AP42"/>
+  <dimension ref="C4:AP46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
     <col min="12" max="12" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
@@ -8065,7 +8084,7 @@
     <col min="29" max="29" width="12.140625" customWidth="1"/>
     <col min="32" max="32" width="13.140625" customWidth="1"/>
     <col min="38" max="38" width="13.140625" customWidth="1"/>
-    <col min="40" max="40" width="12" customWidth="1"/>
+    <col min="39" max="40" width="12" customWidth="1"/>
     <col min="42" max="42" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8186,7 +8205,7 @@
     </row>
     <row r="5" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>51</v>
@@ -8248,60 +8267,60 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1">
-        <v>-47</v>
+        <v>3578</v>
       </c>
       <c r="AA5" s="1">
-        <v>40333</v>
+        <v>47423</v>
       </c>
       <c r="AB5" s="1">
-        <v>4741</v>
+        <v>16239</v>
       </c>
       <c r="AC5" s="1">
-        <v>19539.2</v>
+        <v>37980</v>
       </c>
       <c r="AD5" s="1">
-        <v>14187.05</v>
+        <v>25765</v>
       </c>
       <c r="AE5" s="1">
-        <v>428</v>
+        <v>1125</v>
       </c>
       <c r="AF5" s="1">
-        <v>216727.5</v>
+        <v>2514578</v>
       </c>
       <c r="AG5" s="1">
-        <v>27.2</v>
+        <v>38.1</v>
       </c>
       <c r="AH5" s="1">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="AI5" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AJ5" s="1">
-        <v>416.7</v>
+        <v>569.79999999999995</v>
       </c>
       <c r="AK5" s="1">
-        <v>89856</v>
+        <v>16799</v>
       </c>
       <c r="AL5" s="1">
-        <v>37840.800000000003</v>
+        <v>130765.6</v>
       </c>
       <c r="AM5" s="1">
-        <v>3314161</v>
+        <v>6645414.4000000004</v>
       </c>
       <c r="AN5" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AO5" s="1">
-        <v>936</v>
+        <v>2690</v>
       </c>
       <c r="AP5" s="1">
-        <v>4090149.6</v>
+        <v>41419617.100000001</v>
       </c>
     </row>
     <row r="6" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>52</v>
@@ -8375,10 +8394,14 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
     </row>
     <row r="7" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>67</v>
@@ -8441,68 +8464,68 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1">
+      <c r="AB7" s="24">
         <f>AB5/$AA5</f>
-        <v>0.11754642600352069</v>
+        <v>0.34242877928431353</v>
       </c>
       <c r="AC7" s="1">
-        <v>19539.2</v>
-      </c>
-      <c r="AD7" s="1">
-        <f t="shared" ref="AD7:AP7" si="0">AD5/$AA5</f>
-        <v>0.35174794833015149</v>
-      </c>
-      <c r="AE7" s="1">
+        <v>37980</v>
+      </c>
+      <c r="AD7" s="24">
+        <f t="shared" ref="AC7:AP7" si="0">AD5/$AA5</f>
+        <v>0.54330177340109231</v>
+      </c>
+      <c r="AE7" s="24">
         <f t="shared" si="0"/>
-        <v>1.0611657947586344E-2</v>
-      </c>
-      <c r="AF7" s="1">
+        <v>2.3722666216814625E-2</v>
+      </c>
+      <c r="AF7" s="24">
         <f t="shared" si="0"/>
-        <v>5.3734534996156995</v>
+        <v>53.024439617906921</v>
       </c>
       <c r="AG7" s="1">
-        <v>27.2</v>
-      </c>
-      <c r="AH7" s="1">
+        <v>38.1</v>
+      </c>
+      <c r="AH7" s="24">
         <f t="shared" si="0"/>
-        <v>3.0991991669352638E-3</v>
-      </c>
-      <c r="AI7" s="1">
+        <v>3.6901925226156085E-3</v>
+      </c>
+      <c r="AI7" s="24">
         <f t="shared" si="0"/>
-        <v>1.2892668534450699E-3</v>
-      </c>
-      <c r="AJ7" s="1">
+        <v>1.1176011639921558E-3</v>
+      </c>
+      <c r="AJ7" s="24">
         <f t="shared" si="0"/>
-        <v>1.0331490342895395E-2</v>
-      </c>
-      <c r="AK7" s="1">
+        <v>1.201526685363642E-2</v>
+      </c>
+      <c r="AK7" s="24">
         <f t="shared" si="0"/>
-        <v>2.2278531227530807</v>
-      </c>
-      <c r="AL7" s="1">
+        <v>0.35423739535668347</v>
+      </c>
+      <c r="AL7" s="24">
         <f t="shared" si="0"/>
-        <v>0.93820940668931152</v>
-      </c>
-      <c r="AM7" s="1">
+        <v>2.7574299390591066</v>
+      </c>
+      <c r="AM7" s="24">
         <f t="shared" si="0"/>
-        <v>82.169960082314731</v>
-      </c>
-      <c r="AN7" s="1">
+        <v>140.13062016321194</v>
+      </c>
+      <c r="AN7" s="24">
         <f t="shared" si="0"/>
-        <v>7.9339498673542752E-4</v>
-      </c>
-      <c r="AO7" s="1">
+        <v>8.8564620542774602E-4</v>
+      </c>
+      <c r="AO7" s="24">
         <f t="shared" si="0"/>
-        <v>2.3206803362011256E-2</v>
-      </c>
-      <c r="AP7" s="1">
+        <v>5.6723530776205636E-2</v>
+      </c>
+      <c r="AP7" s="24">
         <f t="shared" si="0"/>
-        <v>101.40950586368483</v>
+        <v>873.40777892583776</v>
       </c>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>68</v>
@@ -8577,6 +8600,68 @@
       <c r="AJ8" s="13"/>
       <c r="AK8" s="13"/>
       <c r="AL8" s="13"/>
+    </row>
+    <row r="9" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3578</v>
+      </c>
+      <c r="G9" s="1">
+        <v>47423</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.34242877928431353</v>
+      </c>
+      <c r="I9" s="7">
+        <v>37980</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.54330177340109231</v>
+      </c>
+      <c r="K9" s="7">
+        <v>2.3722666216814625E-2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>53.024439617906921</v>
+      </c>
+      <c r="M9" s="7">
+        <v>38.1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>3.6901925226156085E-3</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1.1176011639921558E-3</v>
+      </c>
+      <c r="P9" s="7">
+        <v>1.201526685363642E-2</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>0.35423739535668347</v>
+      </c>
+      <c r="R9" s="7">
+        <v>2.7574299390591066</v>
+      </c>
+      <c r="S9" s="7">
+        <v>140.13062016321194</v>
+      </c>
+      <c r="T9" s="7">
+        <v>8.8564620542774602E-4</v>
+      </c>
+      <c r="U9" s="7">
+        <v>5.6723530776205636E-2</v>
+      </c>
+      <c r="V9" s="7">
+        <v>873.40777892583776</v>
+      </c>
     </row>
     <row r="10" spans="3:42" x14ac:dyDescent="0.25">
       <c r="V10" s="1"/>
@@ -8598,60 +8683,6 @@
       <c r="AL10" s="1"/>
     </row>
     <row r="12" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -8669,124 +8700,68 @@
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
     </row>
-    <row r="13" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
-        <v>80631000</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G13" s="7">
-        <v>5.713E-2</v>
-      </c>
-      <c r="H13" s="7">
-        <v>6.6350000000000006E-2</v>
-      </c>
-      <c r="I13" s="7">
-        <v>6.54E-2</v>
-      </c>
-      <c r="J13" s="7">
-        <v>4.7969999999999999E-2</v>
-      </c>
-      <c r="K13" s="7">
-        <v>4.8160000000000001E-2</v>
-      </c>
-      <c r="L13" s="7">
-        <v>4.5749999999999999E-2</v>
-      </c>
-      <c r="M13" s="7">
-        <v>7.306E-2</v>
-      </c>
-      <c r="N13" s="7">
-        <v>7.0499999999999993E-2</v>
-      </c>
-      <c r="O13" s="7">
-        <v>6.5699999999999995E-2</v>
-      </c>
-      <c r="P13" s="7">
-        <v>6.1429999999999998E-2</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>0.14660000000000001</v>
-      </c>
-      <c r="R13" s="7">
-        <v>9.0639999999999998E-2</v>
-      </c>
-      <c r="S13" s="7">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="T13" s="7">
-        <v>7.3700000000000002E-2</v>
-      </c>
-    </row>
     <row r="14" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
-        <v>80631000</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G14" s="7">
-        <v>6.1899999999999997E-2</v>
-      </c>
-      <c r="H14" s="7">
-        <v>7.1800000000000003E-2</v>
-      </c>
-      <c r="I14" s="7">
-        <v>6.9099999999999995E-2</v>
-      </c>
-      <c r="J14" s="7">
-        <v>5.1240000000000001E-2</v>
-      </c>
-      <c r="K14" s="7">
-        <v>4.446E-2</v>
-      </c>
-      <c r="L14" s="7">
-        <v>8.0439999999999998E-2</v>
-      </c>
-      <c r="M14" s="7">
-        <v>9.3899999999999997E-2</v>
-      </c>
-      <c r="N14" s="7">
-        <v>7.5130000000000002E-2</v>
-      </c>
-      <c r="O14" s="7">
-        <v>6.3600000000000004E-2</v>
-      </c>
-      <c r="P14" s="7">
-        <v>6.1039999999999997E-2</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>0.1278</v>
-      </c>
-      <c r="R14" s="7">
-        <v>7.6969999999999997E-2</v>
-      </c>
-      <c r="S14" s="7">
-        <v>7.2900000000000006E-2</v>
-      </c>
-      <c r="T14" s="7">
-        <v>4.9840000000000002E-2</v>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
-        <v>80601000</v>
+        <v>80631000</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>41</v>
@@ -8795,54 +8770,54 @@
         <v>2020</v>
       </c>
       <c r="G15" s="7">
-        <v>7.2270000000000001E-2</v>
+        <v>5.713E-2</v>
       </c>
       <c r="H15" s="7">
-        <v>8.7160000000000001E-2</v>
+        <v>6.6350000000000006E-2</v>
       </c>
       <c r="I15" s="7">
-        <v>8.0140000000000003E-2</v>
+        <v>6.54E-2</v>
       </c>
       <c r="J15" s="7">
-        <v>5.5300000000000002E-2</v>
+        <v>4.7969999999999999E-2</v>
       </c>
       <c r="K15" s="7">
-        <v>5.79E-2</v>
+        <v>4.8160000000000001E-2</v>
       </c>
       <c r="L15" s="7">
-        <v>4.1930000000000002E-2</v>
+        <v>4.5749999999999999E-2</v>
       </c>
       <c r="M15" s="7">
-        <v>6.9599999999999995E-2</v>
+        <v>7.306E-2</v>
       </c>
       <c r="N15" s="7">
-        <v>6.2469999999999998E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="O15" s="7">
-        <v>6.2560000000000004E-2</v>
+        <v>6.5699999999999995E-2</v>
       </c>
       <c r="P15" s="7">
-        <v>5.91E-2</v>
+        <v>6.1429999999999998E-2</v>
       </c>
       <c r="Q15" s="7">
-        <v>0.14610000000000001</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="R15" s="7">
-        <v>8.5139999999999993E-2</v>
+        <v>9.0639999999999998E-2</v>
       </c>
       <c r="S15" s="7">
-        <v>7.1900000000000006E-2</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="T15" s="7">
-        <v>4.8500000000000001E-2</v>
+        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
-        <v>80601000</v>
+        <v>80631000</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>42</v>
@@ -8851,1140 +8826,1376 @@
         <v>2020</v>
       </c>
       <c r="G16" s="7">
-        <v>7.2139999999999996E-2</v>
+        <v>6.1899999999999997E-2</v>
       </c>
       <c r="H16" s="7">
-        <v>8.6360000000000006E-2</v>
+        <v>7.1800000000000003E-2</v>
       </c>
       <c r="I16" s="7">
-        <v>8.2460000000000006E-2</v>
+        <v>6.9099999999999995E-2</v>
       </c>
       <c r="J16" s="7">
-        <v>5.8470000000000001E-2</v>
+        <v>5.1240000000000001E-2</v>
       </c>
       <c r="K16" s="7">
-        <v>6.5250000000000002E-2</v>
+        <v>4.446E-2</v>
       </c>
       <c r="L16" s="7">
-        <v>5.7099999999999998E-2</v>
+        <v>8.0439999999999998E-2</v>
       </c>
       <c r="M16" s="7">
-        <v>8.0140000000000003E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="N16" s="7">
-        <v>7.0860000000000006E-2</v>
+        <v>7.5130000000000002E-2</v>
       </c>
       <c r="O16" s="7">
-        <v>5.8900000000000001E-2</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="P16" s="7">
-        <v>5.8779999999999999E-2</v>
+        <v>6.1039999999999997E-2</v>
       </c>
       <c r="Q16" s="7">
-        <v>0.1333</v>
+        <v>0.1278</v>
       </c>
       <c r="R16" s="7">
-        <v>7.9000000000000001E-2</v>
+        <v>7.6969999999999997E-2</v>
       </c>
       <c r="S16" s="7">
-        <v>6.1650000000000003E-2</v>
+        <v>7.2900000000000006E-2</v>
       </c>
       <c r="T16" s="7">
-        <v>3.5639999999999998E-2</v>
+        <v>4.9840000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
-        <v>38701000</v>
+        <v>80601000</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="G17" s="7">
-        <v>4.2900000000000001E-2</v>
+        <v>7.2270000000000001E-2</v>
       </c>
       <c r="H17" s="7">
-        <v>5.9499999999999997E-2</v>
+        <v>8.7160000000000001E-2</v>
       </c>
       <c r="I17" s="7">
-        <v>5.475E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="J17" s="7">
-        <v>4.8550000000000003E-2</v>
+        <v>5.5300000000000002E-2</v>
       </c>
       <c r="K17" s="7">
-        <v>4.48E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="L17" s="7">
-        <v>4.9930000000000002E-2</v>
+        <v>4.1930000000000002E-2</v>
       </c>
       <c r="M17" s="7">
-        <v>7.6899999999999996E-2</v>
+        <v>6.9599999999999995E-2</v>
       </c>
       <c r="N17" s="7">
-        <v>9.2039999999999997E-2</v>
+        <v>6.2469999999999998E-2</v>
       </c>
       <c r="O17" s="7">
-        <v>8.1799999999999998E-2</v>
+        <v>6.2560000000000004E-2</v>
       </c>
       <c r="P17" s="7">
-        <v>7.6100000000000001E-2</v>
+        <v>5.91E-2</v>
       </c>
       <c r="Q17" s="7">
-        <v>0.12427000000000001</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="R17" s="7">
-        <v>7.0400000000000004E-2</v>
+        <v>8.5139999999999993E-2</v>
       </c>
       <c r="S17" s="7">
-        <v>9.0700000000000003E-2</v>
+        <v>7.1900000000000006E-2</v>
       </c>
       <c r="T17" s="7">
-        <v>8.7340000000000001E-2</v>
+        <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
-        <v>38701000</v>
+        <v>80601000</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="G18" s="7">
-        <v>5.4960000000000002E-2</v>
+        <v>7.2139999999999996E-2</v>
       </c>
       <c r="H18" s="7">
-        <v>7.3400000000000007E-2</v>
+        <v>8.6360000000000006E-2</v>
       </c>
       <c r="I18" s="7">
-        <v>6.744E-2</v>
+        <v>8.2460000000000006E-2</v>
       </c>
       <c r="J18" s="7">
-        <v>6.1460000000000001E-2</v>
+        <v>5.8470000000000001E-2</v>
       </c>
       <c r="K18" s="7">
-        <v>4.82E-2</v>
+        <v>6.5250000000000002E-2</v>
       </c>
       <c r="L18" s="7">
-        <v>5.2060000000000002E-2</v>
+        <v>5.7099999999999998E-2</v>
       </c>
       <c r="M18" s="7">
-        <v>7.9200000000000007E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="N18" s="7">
-        <v>9.7000000000000003E-2</v>
+        <v>7.0860000000000006E-2</v>
       </c>
       <c r="O18" s="7">
-        <v>8.4839999999999999E-2</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="P18" s="7">
-        <v>7.6100000000000001E-2</v>
+        <v>5.8779999999999999E-2</v>
       </c>
       <c r="Q18" s="7">
-        <v>0.11269999999999999</v>
+        <v>0.1333</v>
       </c>
       <c r="R18" s="7">
-        <v>6.1600000000000002E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="S18" s="7">
-        <v>7.1529999999999996E-2</v>
+        <v>6.1650000000000003E-2</v>
       </c>
       <c r="T18" s="7">
-        <v>5.9630000000000002E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
-        <v>20627000</v>
+        <v>38701000</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="1">
-        <v>2012</v>
+        <v>2023</v>
       </c>
       <c r="G19" s="7">
-        <v>5.9569999999999998E-2</v>
+        <v>4.2900000000000001E-2</v>
       </c>
       <c r="H19" s="7">
-        <v>5.3039999999999997E-2</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="I19" s="7">
-        <v>5.57E-2</v>
+        <v>5.475E-2</v>
       </c>
       <c r="J19" s="7">
-        <v>5.1450000000000003E-2</v>
+        <v>4.8550000000000003E-2</v>
       </c>
       <c r="K19" s="7">
-        <v>6.5369999999999998E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="L19" s="7">
-        <v>7.7899999999999997E-2</v>
+        <v>4.9930000000000002E-2</v>
       </c>
       <c r="M19" s="7">
         <v>7.6899999999999996E-2</v>
       </c>
       <c r="N19" s="7">
-        <v>7.6999999999999999E-2</v>
+        <v>9.2039999999999997E-2</v>
       </c>
       <c r="O19" s="7">
-        <v>7.4999999999999997E-2</v>
+        <v>8.1799999999999998E-2</v>
       </c>
       <c r="P19" s="7">
-        <v>8.6099999999999996E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="Q19" s="7">
-        <v>0.10284</v>
+        <v>0.12427000000000001</v>
       </c>
       <c r="R19" s="7">
-        <v>8.9099999999999999E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="S19" s="7">
-        <v>8.5599999999999996E-2</v>
+        <v>9.0700000000000003E-2</v>
       </c>
       <c r="T19" s="7">
-        <v>4.4400000000000002E-2</v>
+        <v>8.7340000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <v>20627000</v>
+        <v>38701000</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G20" s="7">
+        <v>5.4960000000000002E-2</v>
+      </c>
+      <c r="H20" s="7">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="I20" s="7">
+        <v>6.744E-2</v>
+      </c>
+      <c r="J20" s="7">
+        <v>6.1460000000000001E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <v>4.82E-2</v>
+      </c>
+      <c r="L20" s="7">
+        <v>5.2060000000000002E-2</v>
+      </c>
+      <c r="M20" s="7">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="N20" s="7">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="O20" s="7">
+        <v>8.4839999999999999E-2</v>
+      </c>
+      <c r="P20" s="7">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0.11269999999999999</v>
+      </c>
+      <c r="R20" s="7">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="S20" s="7">
+        <v>7.1529999999999996E-2</v>
+      </c>
+      <c r="T20" s="7">
+        <v>5.9630000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>20627000</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
         <v>2012</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G21" s="7">
+        <v>5.9569999999999998E-2</v>
+      </c>
+      <c r="H21" s="7">
+        <v>5.3039999999999997E-2</v>
+      </c>
+      <c r="I21" s="7">
+        <v>5.57E-2</v>
+      </c>
+      <c r="J21" s="7">
+        <v>5.1450000000000003E-2</v>
+      </c>
+      <c r="K21" s="7">
+        <v>6.5369999999999998E-2</v>
+      </c>
+      <c r="L21" s="7">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="M21" s="7">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="N21" s="7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O21" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P21" s="7">
+        <v>8.6099999999999996E-2</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.10284</v>
+      </c>
+      <c r="R21" s="7">
+        <v>8.9099999999999999E-2</v>
+      </c>
+      <c r="S21" s="7">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="T21" s="7">
+        <v>4.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>20627000</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2012</v>
+      </c>
+      <c r="G22" s="7">
         <v>6.1280000000000001E-2</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H22" s="7">
         <v>5.9360000000000003E-2</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I22" s="7">
         <v>6.4899999999999999E-2</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J22" s="7">
         <v>6.3600000000000004E-2</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K22" s="7">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L22" s="7">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M22" s="7">
         <v>7.6700000000000004E-2</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N22" s="7">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O22" s="7">
         <v>7.4300000000000005E-2</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P22" s="7">
         <v>8.6300000000000002E-2</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q22" s="7">
         <v>0.10297000000000001</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R22" s="7">
         <v>8.0699999999999994E-2</v>
       </c>
-      <c r="S20" s="7">
+      <c r="S22" s="7">
         <v>6.6650000000000001E-2</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T22" s="7">
         <v>2.6980000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D23" s="3" t="s">
-        <v>43</v>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>92634000</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="G23" s="7">
-        <f>AVERAGE(G13,G15,G17,G19)</f>
-        <v>5.7967500000000005E-2</v>
+        <v>6.1769999999999999E-2</v>
       </c>
       <c r="H23" s="7">
-        <f t="shared" ref="H23:T23" si="1">AVERAGE(H13,H15,H17,H19)</f>
-        <v>6.6512500000000002E-2</v>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" si="1"/>
-        <v>6.3997499999999999E-2</v>
+        <v>5.21E-2</v>
       </c>
       <c r="J23" s="7">
-        <f t="shared" si="1"/>
-        <v>5.0817500000000002E-2</v>
+        <v>4.675E-2</v>
       </c>
       <c r="K23" s="7">
-        <f t="shared" si="1"/>
-        <v>5.4057499999999994E-2</v>
+        <v>4.8070000000000002E-2</v>
       </c>
       <c r="L23" s="7">
-        <f t="shared" si="1"/>
-        <v>5.3877500000000002E-2</v>
+        <v>7.0599999999999996E-2</v>
       </c>
       <c r="M23" s="7">
-        <f t="shared" si="1"/>
-        <v>7.4115E-2</v>
+        <v>9.35E-2</v>
       </c>
       <c r="N23" s="7">
-        <f t="shared" si="1"/>
-        <v>7.55025E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" si="1"/>
-        <v>7.1264999999999995E-2</v>
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="P23" s="7">
-        <f t="shared" si="1"/>
-        <v>7.0682499999999995E-2</v>
+        <v>5.9080000000000001E-2</v>
       </c>
       <c r="Q23" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1299525</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="R23" s="7">
-        <f t="shared" si="1"/>
-        <v>8.3820000000000006E-2</v>
+        <v>7.7759999999999996E-2</v>
       </c>
       <c r="S23" s="7">
-        <f t="shared" si="1"/>
-        <v>8.3925E-2</v>
+        <v>8.4659999999999999E-2</v>
       </c>
       <c r="T23" s="7">
-        <f t="shared" si="1"/>
-        <v>6.3485E-2</v>
+        <v>6.1519999999999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D24" s="3" t="s">
-        <v>43</v>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>92634000</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G24" s="7">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="H24" s="7">
+        <v>7.6050000000000006E-2</v>
+      </c>
+      <c r="I24" s="7">
+        <v>5.7860000000000002E-2</v>
+      </c>
+      <c r="J24" s="7">
+        <v>4.8829999999999998E-2</v>
+      </c>
+      <c r="K24" s="7">
+        <v>4.376E-2</v>
+      </c>
+      <c r="L24" s="7">
+        <v>7.7299999999999994E-2</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0.10564999999999999</v>
+      </c>
+      <c r="N24" s="7">
+        <v>8.0750000000000002E-2</v>
+      </c>
+      <c r="O24" s="7">
+        <v>7.22E-2</v>
+      </c>
+      <c r="P24" s="7">
+        <v>5.8779999999999999E-2</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="R24" s="7">
+        <v>7.0739999999999997E-2</v>
+      </c>
+      <c r="S24" s="7">
+        <v>7.2139999999999996E-2</v>
+      </c>
+      <c r="T24" s="7">
+        <v>4.9160000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="1">
         <v>0</v>
       </c>
-      <c r="G24" s="7">
-        <f>AVERAGE(G14,G16,G18,G20)</f>
+      <c r="G27" s="7">
+        <f>AVERAGE(G15,G17,G19,G21)</f>
+        <v>5.7967500000000005E-2</v>
+      </c>
+      <c r="H27" s="7">
+        <f>AVERAGE(H15,H17,H19,H21)</f>
+        <v>6.6512500000000002E-2</v>
+      </c>
+      <c r="I27" s="7">
+        <f>AVERAGE(I15,I17,I19,I21)</f>
+        <v>6.3997499999999999E-2</v>
+      </c>
+      <c r="J27" s="7">
+        <f>AVERAGE(J15,J17,J19,J21)</f>
+        <v>5.0817500000000002E-2</v>
+      </c>
+      <c r="K27" s="7">
+        <f>AVERAGE(K15,K17,K19,K21)</f>
+        <v>5.4057499999999994E-2</v>
+      </c>
+      <c r="L27" s="7">
+        <f>AVERAGE(L15,L17,L19,L21)</f>
+        <v>5.3877500000000002E-2</v>
+      </c>
+      <c r="M27" s="7">
+        <f>AVERAGE(M15,M17,M19,M21)</f>
+        <v>7.4115E-2</v>
+      </c>
+      <c r="N27" s="7">
+        <f>AVERAGE(N15,N17,N19,N21)</f>
+        <v>7.55025E-2</v>
+      </c>
+      <c r="O27" s="7">
+        <f>AVERAGE(O15,O17,O19,O21)</f>
+        <v>7.1264999999999995E-2</v>
+      </c>
+      <c r="P27" s="7">
+        <f>AVERAGE(P15,P17,P19,P21)</f>
+        <v>7.0682499999999995E-2</v>
+      </c>
+      <c r="Q27" s="7">
+        <f>AVERAGE(Q15,Q17,Q19,Q21)</f>
+        <v>0.1299525</v>
+      </c>
+      <c r="R27" s="7">
+        <f>AVERAGE(R15,R17,R19,R21)</f>
+        <v>8.3820000000000006E-2</v>
+      </c>
+      <c r="S27" s="7">
+        <f>AVERAGE(S15,S17,S19,S21)</f>
+        <v>8.3925E-2</v>
+      </c>
+      <c r="T27" s="7">
+        <f>AVERAGE(T15,T17,T19,T21)</f>
+        <v>6.3485E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <f>AVERAGE(G16,G18,G20,G22)</f>
         <v>6.2570000000000001E-2</v>
       </c>
-      <c r="H24" s="7">
-        <f t="shared" ref="H24:T24" si="2">AVERAGE(H14,H16,H18,H20)</f>
+      <c r="H28" s="7">
+        <f>AVERAGE(H16,H18,H20,H22)</f>
         <v>7.2730000000000017E-2</v>
       </c>
-      <c r="I24" s="7">
-        <f t="shared" si="2"/>
+      <c r="I28" s="7">
+        <f>AVERAGE(I16,I18,I20,I22)</f>
         <v>7.0974999999999996E-2</v>
       </c>
-      <c r="J24" s="7">
-        <f t="shared" si="2"/>
+      <c r="J28" s="7">
+        <f>AVERAGE(J16,J18,J20,J22)</f>
         <v>5.8692499999999995E-2</v>
       </c>
-      <c r="K24" s="7">
-        <f t="shared" si="2"/>
+      <c r="K28" s="7">
+        <f>AVERAGE(K16,K18,K20,K22)</f>
         <v>5.7327500000000003E-2</v>
       </c>
-      <c r="L24" s="7">
-        <f t="shared" si="2"/>
+      <c r="L28" s="7">
+        <f>AVERAGE(L16,L18,L20,L22)</f>
         <v>6.9550000000000001E-2</v>
       </c>
-      <c r="M24" s="7">
-        <f t="shared" si="2"/>
+      <c r="M28" s="7">
+        <f>AVERAGE(M16,M18,M20,M22)</f>
         <v>8.2485000000000003E-2</v>
       </c>
-      <c r="N24" s="7">
-        <f t="shared" si="2"/>
+      <c r="N28" s="7">
+        <f>AVERAGE(N16,N18,N20,N22)</f>
         <v>7.9822500000000005E-2</v>
       </c>
-      <c r="O24" s="7">
-        <f t="shared" si="2"/>
+      <c r="O28" s="7">
+        <f>AVERAGE(O16,O18,O20,O22)</f>
         <v>7.041E-2</v>
       </c>
-      <c r="P24" s="7">
-        <f t="shared" si="2"/>
+      <c r="P28" s="7">
+        <f>AVERAGE(P16,P18,P20,P22)</f>
         <v>7.0554999999999993E-2</v>
       </c>
-      <c r="Q24" s="7">
-        <f t="shared" si="2"/>
+      <c r="Q28" s="7">
+        <f>AVERAGE(Q16,Q18,Q20,Q22)</f>
         <v>0.11919250000000001</v>
       </c>
-      <c r="R24" s="7">
-        <f t="shared" si="2"/>
+      <c r="R28" s="7">
+        <f>AVERAGE(R16,R18,R20,R22)</f>
         <v>7.4567499999999995E-2</v>
       </c>
-      <c r="S24" s="7">
-        <f t="shared" si="2"/>
+      <c r="S28" s="7">
+        <f>AVERAGE(S16,S18,S20,S22)</f>
         <v>6.8182499999999993E-2</v>
       </c>
-      <c r="T24" s="7">
-        <f t="shared" si="2"/>
+      <c r="T28" s="7">
+        <f>AVERAGE(T16,T18,T20,T22)</f>
         <v>4.3022500000000005E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V29" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2015</v>
-      </c>
-      <c r="F30" s="1">
-        <v>-508</v>
-      </c>
-      <c r="G30" s="1">
-        <v>89673</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0.17097677115742749</v>
-      </c>
-      <c r="I30" s="1">
-        <v>20274.726180000001</v>
-      </c>
-      <c r="J30" s="1">
-        <v>0.63144982324668508</v>
-      </c>
-      <c r="K30" s="1">
-        <v>1.8846252495176911E-2</v>
-      </c>
-      <c r="L30" s="1">
-        <v>23.73828289719313</v>
-      </c>
-      <c r="M30" s="1">
-        <v>25.6</v>
-      </c>
-      <c r="N30" s="1">
-        <v>5.8769083224604586E-3</v>
-      </c>
-      <c r="O30" s="1">
-        <v>2.9663332329686628E-3</v>
-      </c>
-      <c r="P30" s="1">
-        <v>8.227671651444687E-3</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>1.0814961025057701</v>
-      </c>
-      <c r="R30" s="1">
-        <v>0.67026351298607134</v>
-      </c>
-      <c r="S30" s="1">
-        <v>25.881326426014489</v>
-      </c>
-      <c r="T30" s="1">
-        <v>4.9067166259632105E-4</v>
-      </c>
-      <c r="U30" s="1">
-        <v>5.6929064489868737E-2</v>
-      </c>
-      <c r="V30" s="1">
-        <v>119.345016326319</v>
-      </c>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F31" s="1">
-        <v>-583</v>
-      </c>
-      <c r="G31" s="1">
-        <v>88968</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0.1689259059437101</v>
-      </c>
-      <c r="I31" s="1">
-        <v>21016.71081</v>
-      </c>
-      <c r="J31" s="1">
-        <v>0.63645580433414262</v>
-      </c>
-      <c r="K31" s="1">
-        <v>1.899559392140994E-2</v>
-      </c>
-      <c r="L31" s="1">
-        <v>23.527577473473599</v>
-      </c>
-      <c r="M31" s="1">
-        <v>26.6</v>
-      </c>
-      <c r="N31" s="1">
-        <v>5.9234781044869714E-3</v>
-      </c>
-      <c r="O31" s="1">
-        <v>3.0572790216706999E-3</v>
-      </c>
-      <c r="P31" s="1">
-        <v>8.4412372988040517E-3</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>1.082479093606689</v>
-      </c>
-      <c r="R31" s="1">
-        <v>0.61311033180469354</v>
-      </c>
-      <c r="S31" s="1">
-        <v>24.770910734196551</v>
-      </c>
-      <c r="T31" s="1">
-        <v>4.9455984174084965E-4</v>
-      </c>
-      <c r="U31" s="1">
-        <v>5.7874741480082717E-2</v>
-      </c>
-      <c r="V31" s="1">
-        <v>143.61354485994971</v>
-      </c>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2017</v>
-      </c>
-      <c r="F32" s="1">
-        <v>-507</v>
-      </c>
-      <c r="G32" s="1">
-        <v>88092</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0.1657471734096172</v>
-      </c>
-      <c r="I32" s="1">
-        <v>22275.830239999999</v>
-      </c>
-      <c r="J32" s="1">
-        <v>0.67765063796939562</v>
-      </c>
-      <c r="K32" s="1">
-        <v>1.9740725605049251E-2</v>
-      </c>
-      <c r="L32" s="1">
-        <v>26.707001895631841</v>
-      </c>
-      <c r="M32" s="1">
-        <v>27.4</v>
-      </c>
-      <c r="N32" s="1">
-        <v>5.9823820551241514E-3</v>
-      </c>
-      <c r="O32" s="1">
-        <v>3.0536257548926002E-3</v>
-      </c>
-      <c r="P32" s="1">
-        <v>8.7851337238341615E-3</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>1.0234073468646401</v>
-      </c>
-      <c r="R32" s="1">
-        <v>0.61994051673250683</v>
-      </c>
-      <c r="S32" s="1">
-        <v>21.178866225082849</v>
-      </c>
-      <c r="T32" s="1">
-        <v>4.9947781864414359E-4</v>
-      </c>
-      <c r="U32" s="1">
-        <v>5.87113472278981E-2</v>
-      </c>
-      <c r="V32" s="1">
-        <v>142.04406721007581</v>
       </c>
     </row>
     <row r="33" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F33" s="1">
-        <v>-711</v>
-      </c>
-      <c r="G33" s="1">
-        <v>87282</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0.16122453655965721</v>
-      </c>
-      <c r="I33" s="1">
-        <v>23989.908439999999</v>
-      </c>
-      <c r="J33" s="1">
-        <v>0.68737654957494088</v>
-      </c>
-      <c r="K33" s="1">
-        <v>1.875529891615681E-2</v>
-      </c>
-      <c r="L33" s="1">
-        <v>29.351305275772781</v>
-      </c>
-      <c r="M33" s="1">
-        <v>28.1</v>
-      </c>
-      <c r="N33" s="1">
-        <v>6.3586993881899652E-3</v>
-      </c>
-      <c r="O33" s="1">
-        <v>3.0819642079695569E-3</v>
-      </c>
-      <c r="P33" s="1">
-        <v>9.3810865928828282E-3</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>0.98409752297151609</v>
-      </c>
-      <c r="R33" s="1">
-        <v>0.71611913109232095</v>
-      </c>
-      <c r="S33" s="1">
-        <v>20.416691414037231</v>
-      </c>
-      <c r="T33" s="1">
-        <v>5.0411310464929633E-4</v>
-      </c>
-      <c r="U33" s="1">
-        <v>5.925620402832199E-2</v>
-      </c>
-      <c r="V33" s="1">
-        <v>145.038276238858</v>
+      <c r="C33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="3">
-        <v>2020</v>
+      <c r="E34" s="1">
+        <v>2015</v>
       </c>
       <c r="F34" s="1">
-        <v>-151.99999999999989</v>
+        <v>-508</v>
       </c>
       <c r="G34" s="1">
-        <v>85939</v>
+        <v>89673</v>
       </c>
       <c r="H34" s="1">
-        <v>0.15749543280699099</v>
+        <v>0.17097677115742749</v>
       </c>
       <c r="I34" s="1">
-        <v>24720.091919999999</v>
+        <v>20274.726180000001</v>
       </c>
       <c r="J34" s="1">
-        <v>0.81039690943576237</v>
+        <v>0.63144982324668508</v>
       </c>
       <c r="K34" s="1">
-        <v>1.8396769801836171E-2</v>
+        <v>1.8846252495176911E-2</v>
       </c>
       <c r="L34" s="1">
-        <v>32.194688077822633</v>
+        <v>23.73828289719313</v>
       </c>
       <c r="M34" s="1">
-        <v>28.7</v>
+        <v>25.6</v>
       </c>
       <c r="N34" s="1">
-        <v>6.539522219248496E-3</v>
+        <v>5.8769083224604586E-3</v>
       </c>
       <c r="O34" s="1">
-        <v>2.5715914776760149E-3</v>
+        <v>2.9663332329686628E-3</v>
       </c>
       <c r="P34" s="1">
-        <v>1.0555161219004169E-2</v>
+        <v>8.227671651444687E-3</v>
       </c>
       <c r="Q34" s="1">
-        <v>1.1495013905211819</v>
+        <v>1.0814961025057701</v>
       </c>
       <c r="R34" s="1">
-        <v>0.66520904362396571</v>
+        <v>0.67026351298607134</v>
       </c>
       <c r="S34" s="1">
-        <v>22.581482595794672</v>
+        <v>25.881326426014489</v>
       </c>
       <c r="T34" s="1">
-        <v>7.4471427407812321E-4</v>
+        <v>4.9067166259632105E-4</v>
       </c>
       <c r="U34" s="1">
-        <v>6.0112405310743661E-2</v>
+        <v>5.6929064489868737E-2</v>
       </c>
       <c r="V34" s="1">
-        <v>153.74505778284589</v>
+        <v>119.345016326319</v>
+      </c>
+    </row>
+    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-583</v>
+      </c>
+      <c r="G35" s="1">
+        <v>88968</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.1689259059437101</v>
+      </c>
+      <c r="I35" s="1">
+        <v>21016.71081</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.63645580433414262</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1.899559392140994E-2</v>
+      </c>
+      <c r="L35" s="1">
+        <v>23.527577473473599</v>
+      </c>
+      <c r="M35" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="N35" s="1">
+        <v>5.9234781044869714E-3</v>
+      </c>
+      <c r="O35" s="1">
+        <v>3.0572790216706999E-3</v>
+      </c>
+      <c r="P35" s="1">
+        <v>8.4412372988040517E-3</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>1.082479093606689</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0.61311033180469354</v>
+      </c>
+      <c r="S35" s="1">
+        <v>24.770910734196551</v>
+      </c>
+      <c r="T35" s="1">
+        <v>4.9455984174084965E-4</v>
+      </c>
+      <c r="U35" s="1">
+        <v>5.7874741480082717E-2</v>
+      </c>
+      <c r="V35" s="1">
+        <v>143.61354485994971</v>
+      </c>
+    </row>
+    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-507</v>
+      </c>
+      <c r="G36" s="1">
+        <v>88092</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.1657471734096172</v>
+      </c>
+      <c r="I36" s="1">
+        <v>22275.830239999999</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.67765063796939562</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1.9740725605049251E-2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>26.707001895631841</v>
+      </c>
+      <c r="M36" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="N36" s="1">
+        <v>5.9823820551241514E-3</v>
+      </c>
+      <c r="O36" s="1">
+        <v>3.0536257548926002E-3</v>
+      </c>
+      <c r="P36" s="1">
+        <v>8.7851337238341615E-3</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>1.0234073468646401</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0.61994051673250683</v>
+      </c>
+      <c r="S36" s="1">
+        <v>21.178866225082849</v>
+      </c>
+      <c r="T36" s="1">
+        <v>4.9947781864414359E-4</v>
+      </c>
+      <c r="U36" s="1">
+        <v>5.87113472278981E-2</v>
+      </c>
+      <c r="V36" s="1">
+        <v>142.04406721007581</v>
       </c>
     </row>
     <row r="37" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V37" s="2" t="s">
-        <v>16</v>
+      <c r="D37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-711</v>
+      </c>
+      <c r="G37" s="1">
+        <v>87282</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.16122453655965721</v>
+      </c>
+      <c r="I37" s="1">
+        <v>23989.908439999999</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.68737654957494088</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1.875529891615681E-2</v>
+      </c>
+      <c r="L37" s="1">
+        <v>29.351305275772781</v>
+      </c>
+      <c r="M37" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="N37" s="1">
+        <v>6.3586993881899652E-3</v>
+      </c>
+      <c r="O37" s="1">
+        <v>3.0819642079695569E-3</v>
+      </c>
+      <c r="P37" s="1">
+        <v>9.3810865928828282E-3</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0.98409752297151609</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0.71611913109232095</v>
+      </c>
+      <c r="S37" s="1">
+        <v>20.416691414037231</v>
+      </c>
+      <c r="T37" s="1">
+        <v>5.0411310464929633E-4</v>
+      </c>
+      <c r="U37" s="1">
+        <v>5.925620402832199E-2</v>
+      </c>
+      <c r="V37" s="1">
+        <v>145.038276238858</v>
       </c>
     </row>
     <row r="38" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="1">
-        <v>2015</v>
+      <c r="C38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2020</v>
       </c>
       <c r="F38" s="1">
-        <v>-163</v>
+        <v>-151.99999999999989</v>
       </c>
       <c r="G38" s="1">
-        <v>44795</v>
+        <v>85939</v>
       </c>
       <c r="H38" s="1">
-        <v>0.1195669159504409</v>
+        <v>0.15749543280699099</v>
       </c>
       <c r="I38" s="1">
-        <v>19632.524519999999</v>
+        <v>24720.091919999999</v>
       </c>
       <c r="J38" s="1">
-        <v>0.26123004799642802</v>
+        <v>0.81039690943576237</v>
       </c>
       <c r="K38" s="1">
-        <v>3.0717714030583751E-2</v>
+        <v>1.8396769801836171E-2</v>
       </c>
       <c r="L38" s="1">
-        <v>6.8428243203482468</v>
+        <v>32.194688077822633</v>
       </c>
       <c r="M38" s="1">
-        <v>25.4</v>
+        <v>28.7</v>
       </c>
       <c r="N38" s="1">
-        <v>3.415559772295994E-3</v>
+        <v>6.539522219248496E-3</v>
       </c>
       <c r="O38" s="1">
-        <v>2.2993637682777002E-3</v>
+        <v>2.5715914776760149E-3</v>
       </c>
       <c r="P38" s="1">
-        <v>1.320683111954458E-2</v>
+        <v>1.0555161219004169E-2</v>
       </c>
       <c r="Q38" s="1">
-        <v>3.216117870298024</v>
+        <v>1.1495013905211819</v>
       </c>
       <c r="R38" s="1">
-        <v>0.54021386315436981</v>
+        <v>0.66520904362396571</v>
       </c>
       <c r="S38" s="1">
-        <v>65.877446219444096</v>
+        <v>22.581482595794672</v>
       </c>
       <c r="T38" s="1">
-        <v>1.5626744056256249E-3</v>
+        <v>7.4471427407812321E-4</v>
       </c>
       <c r="U38" s="1">
-        <v>4.6790936488447371E-2</v>
+        <v>6.0112405310743661E-2</v>
       </c>
       <c r="V38" s="1">
-        <v>36.086993072441103</v>
-      </c>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F39" s="1">
-        <v>-100</v>
-      </c>
-      <c r="G39" s="1">
-        <v>44888</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0.1251559436820531</v>
-      </c>
-      <c r="I39" s="1">
-        <v>18340.544890000001</v>
-      </c>
-      <c r="J39" s="1">
-        <v>0.37225984672963802</v>
-      </c>
-      <c r="K39" s="1">
-        <v>3.412938870076633E-2</v>
-      </c>
-      <c r="L39" s="1">
-        <v>8.4181796671716178</v>
-      </c>
-      <c r="M39" s="1">
-        <v>27.3</v>
-      </c>
-      <c r="N39" s="1">
-        <v>3.2970949919800181E-3</v>
-      </c>
-      <c r="O39" s="1">
-        <v>2.31687756193191E-3</v>
-      </c>
-      <c r="P39" s="1">
-        <v>1.3460167528069861E-2</v>
-      </c>
-      <c r="Q39" s="1">
-        <v>3.237123507396185</v>
-      </c>
-      <c r="R39" s="1">
-        <v>0.44668731063981459</v>
-      </c>
-      <c r="S39" s="1">
-        <v>65.029295230351053</v>
-      </c>
-      <c r="T39" s="1">
-        <v>1.559436820531096E-3</v>
-      </c>
-      <c r="U39" s="1">
-        <v>4.7696489039386912E-2</v>
-      </c>
-      <c r="V39" s="1">
-        <v>36.327307061575482</v>
-      </c>
-    </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="1">
-        <v>2017</v>
-      </c>
-      <c r="F40" s="1">
-        <v>-179</v>
-      </c>
-      <c r="G40" s="1">
-        <v>44962</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0.1264401049775366</v>
-      </c>
-      <c r="I40" s="1">
-        <v>19591.68519</v>
-      </c>
-      <c r="J40" s="1">
-        <v>0.37287042391352693</v>
-      </c>
-      <c r="K40" s="1">
-        <v>3.0603620835372079E-2</v>
-      </c>
-      <c r="L40" s="1">
-        <v>22.083162368444469</v>
-      </c>
-      <c r="M40" s="1">
-        <v>28.1</v>
-      </c>
-      <c r="N40" s="1">
-        <v>3.6475245763088601E-3</v>
-      </c>
-      <c r="O40" s="1">
-        <v>2.3130643654641599E-3</v>
-      </c>
-      <c r="P40" s="1">
-        <v>1.3724923268537871E-2</v>
-      </c>
-      <c r="Q40" s="1">
-        <v>3.2863529202437611</v>
-      </c>
-      <c r="R40" s="1">
-        <v>0.48064810284240023</v>
-      </c>
-      <c r="S40" s="1">
-        <v>62.958639059650331</v>
-      </c>
-      <c r="T40" s="1">
-        <v>1.5568702459854949E-3</v>
-      </c>
-      <c r="U40" s="1">
-        <v>4.7617988523642192E-2</v>
-      </c>
-      <c r="V40" s="1">
-        <v>38.445424051198778</v>
+        <v>153.74505778284589</v>
       </c>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F41" s="1">
-        <v>-56.99999999999995</v>
-      </c>
-      <c r="G41" s="1">
-        <v>44933.999999999993</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0.1135665642942983</v>
-      </c>
-      <c r="I41" s="1">
-        <v>20641.733639999999</v>
-      </c>
-      <c r="J41" s="1">
-        <v>0.37868206703164631</v>
-      </c>
-      <c r="K41" s="1">
-        <v>3.4984644144745607E-2</v>
-      </c>
-      <c r="L41" s="1">
-        <v>23.389734217296478</v>
-      </c>
-      <c r="M41" s="1">
-        <v>28.8</v>
-      </c>
-      <c r="N41" s="1">
-        <v>3.7165620688120122E-3</v>
-      </c>
-      <c r="O41" s="1">
-        <v>2.2699959941247069E-3</v>
-      </c>
-      <c r="P41" s="1">
-        <v>1.374237770952952E-2</v>
-      </c>
-      <c r="Q41" s="1">
-        <v>2.790626251836025</v>
-      </c>
-      <c r="R41" s="1">
-        <v>0.49644456313704521</v>
-      </c>
-      <c r="S41" s="1">
-        <v>59.326706022165851</v>
-      </c>
-      <c r="T41" s="1">
-        <v>1.491075800062311E-3</v>
-      </c>
-      <c r="U41" s="1">
-        <v>4.775893532736903E-2</v>
-      </c>
-      <c r="V41" s="1">
-        <v>34.524197758490182</v>
+      <c r="C41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="C42" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-163</v>
+      </c>
+      <c r="G42" s="1">
+        <v>44795</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.1195669159504409</v>
+      </c>
+      <c r="I42" s="1">
+        <v>19632.524519999999</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.26123004799642802</v>
+      </c>
+      <c r="K42" s="1">
+        <v>3.0717714030583751E-2</v>
+      </c>
+      <c r="L42" s="1">
+        <v>6.8428243203482468</v>
+      </c>
+      <c r="M42" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="N42" s="1">
+        <v>3.415559772295994E-3</v>
+      </c>
+      <c r="O42" s="1">
+        <v>2.2993637682777002E-3</v>
+      </c>
+      <c r="P42" s="1">
+        <v>1.320683111954458E-2</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>3.216117870298024</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0.54021386315436981</v>
+      </c>
+      <c r="S42" s="1">
+        <v>65.877446219444096</v>
+      </c>
+      <c r="T42" s="1">
+        <v>1.5626744056256249E-3</v>
+      </c>
+      <c r="U42" s="1">
+        <v>4.6790936488447371E-2</v>
+      </c>
+      <c r="V42" s="1">
+        <v>36.086993072441103</v>
+      </c>
+    </row>
+    <row r="43" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-100</v>
+      </c>
+      <c r="G43" s="1">
+        <v>44888</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.1251559436820531</v>
+      </c>
+      <c r="I43" s="1">
+        <v>18340.544890000001</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.37225984672963802</v>
+      </c>
+      <c r="K43" s="1">
+        <v>3.412938870076633E-2</v>
+      </c>
+      <c r="L43" s="1">
+        <v>8.4181796671716178</v>
+      </c>
+      <c r="M43" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3.2970949919800181E-3</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2.31687756193191E-3</v>
+      </c>
+      <c r="P43" s="1">
+        <v>1.3460167528069861E-2</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>3.237123507396185</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0.44668731063981459</v>
+      </c>
+      <c r="S43" s="1">
+        <v>65.029295230351053</v>
+      </c>
+      <c r="T43" s="1">
+        <v>1.559436820531096E-3</v>
+      </c>
+      <c r="U43" s="1">
+        <v>4.7696489039386912E-2</v>
+      </c>
+      <c r="V43" s="1">
+        <v>36.327307061575482</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-179</v>
+      </c>
+      <c r="G44" s="1">
+        <v>44962</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.1264401049775366</v>
+      </c>
+      <c r="I44" s="1">
+        <v>19591.68519</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.37287042391352693</v>
+      </c>
+      <c r="K44" s="1">
+        <v>3.0603620835372079E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <v>22.083162368444469</v>
+      </c>
+      <c r="M44" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="N44" s="1">
+        <v>3.6475245763088601E-3</v>
+      </c>
+      <c r="O44" s="1">
+        <v>2.3130643654641599E-3</v>
+      </c>
+      <c r="P44" s="1">
+        <v>1.3724923268537871E-2</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>3.2863529202437611</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0.48064810284240023</v>
+      </c>
+      <c r="S44" s="1">
+        <v>62.958639059650331</v>
+      </c>
+      <c r="T44" s="1">
+        <v>1.5568702459854949E-3</v>
+      </c>
+      <c r="U44" s="1">
+        <v>4.7617988523642192E-2</v>
+      </c>
+      <c r="V44" s="1">
+        <v>38.445424051198778</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F45" s="1">
+        <v>-56.99999999999995</v>
+      </c>
+      <c r="G45" s="1">
+        <v>44933.999999999993</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.1135665642942983</v>
+      </c>
+      <c r="I45" s="1">
+        <v>20641.733639999999</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.37868206703164631</v>
+      </c>
+      <c r="K45" s="1">
+        <v>3.4984644144745607E-2</v>
+      </c>
+      <c r="L45" s="1">
+        <v>23.389734217296478</v>
+      </c>
+      <c r="M45" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="N45" s="1">
+        <v>3.7165620688120122E-3</v>
+      </c>
+      <c r="O45" s="1">
+        <v>2.2699959941247069E-3</v>
+      </c>
+      <c r="P45" s="1">
+        <v>1.374237770952952E-2</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>2.790626251836025</v>
+      </c>
+      <c r="R45" s="1">
+        <v>0.49644456313704521</v>
+      </c>
+      <c r="S45" s="1">
+        <v>59.326706022165851</v>
+      </c>
+      <c r="T45" s="1">
+        <v>1.491075800062311E-3</v>
+      </c>
+      <c r="U45" s="1">
+        <v>4.775893532736903E-2</v>
+      </c>
+      <c r="V45" s="1">
+        <v>34.524197758490182</v>
+      </c>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="3">
         <v>2020</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F46" s="1">
         <v>-449.99999999999989</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G46" s="1">
         <v>44386</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H46" s="1">
         <v>0.11616275402153831</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I46" s="1">
         <v>21819.183840000002</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J46" s="1">
         <v>0.43312530978236369</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K46" s="1">
         <v>3.4515387734871332E-2</v>
       </c>
-      <c r="L42" s="1">
+      <c r="L46" s="1">
         <v>23.330135132699489</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M46" s="1">
         <v>29.9</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N46" s="1">
         <v>3.807506871536046E-3</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O46" s="1">
         <v>2.343081151714495E-3</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P46" s="1">
         <v>1.4168882079935099E-2</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="Q46" s="1">
         <v>2.863042400756993</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R46" s="1">
         <v>0.49934596494390132</v>
       </c>
-      <c r="S42" s="1">
+      <c r="S46" s="1">
         <v>56.510477592033467</v>
       </c>
-      <c r="T42" s="1">
+      <c r="T46" s="1">
         <v>1.622133105033115E-3</v>
       </c>
-      <c r="U42" s="1">
+      <c r="U46" s="1">
         <v>4.9587707835804067E-2</v>
       </c>
-      <c r="V42" s="1">
+      <c r="V46" s="1">
         <v>33.696300743477607</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I30:I34">
+  <conditionalFormatting sqref="I34:I38">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L34:L38">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -9996,7 +10207,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30:L34">
+  <conditionalFormatting sqref="Q34:Q38">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -10008,7 +10219,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q30:Q34">
+  <conditionalFormatting sqref="R34:R38">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -10020,7 +10231,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R30:R34">
+  <conditionalFormatting sqref="S34:S38">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -10032,7 +10243,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S30:S34">
+  <conditionalFormatting sqref="V34:V38">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -10044,7 +10255,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V30:V34">
+  <conditionalFormatting sqref="I42:I46">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -10056,7 +10267,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:I42">
+  <conditionalFormatting sqref="L42:L46">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -10068,7 +10279,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L42">
+  <conditionalFormatting sqref="Q42:Q46">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -10080,7 +10291,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q38:Q42">
+  <conditionalFormatting sqref="R42:R46">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -10092,7 +10303,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R38:R42">
+  <conditionalFormatting sqref="S42:S46">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -10104,7 +10315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S38:S42">
+  <conditionalFormatting sqref="V42:V46">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -10116,7 +10327,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V38:V42">
+  <conditionalFormatting sqref="G15:T15">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -10128,7 +10339,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13:T13">
+  <conditionalFormatting sqref="G16:T16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -10140,7 +10351,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:T14">
+  <conditionalFormatting sqref="G17:T17">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -10152,7 +10363,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:T15">
+  <conditionalFormatting sqref="G18:T18">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -10164,7 +10375,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:T16">
+  <conditionalFormatting sqref="G19:T20">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -10176,7 +10387,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:T18">
+  <conditionalFormatting sqref="G21:T22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -10188,7 +10399,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:T20">
+  <conditionalFormatting sqref="G23:T24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -10209,7 +10420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Protests in Gelendzhik and Anapa
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/soc-conflicts analysis.xlsx
+++ b/migforecasting/social conflicts/soc-conflicts analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="76">
   <si>
     <t>saldo</t>
   </si>
@@ -239,6 +239,18 @@
   </si>
   <si>
     <t>Лаишевский МР</t>
+  </si>
+  <si>
+    <t>Анапа</t>
+  </si>
+  <si>
+    <t>Геленджик</t>
+  </si>
+  <si>
+    <t>город-курорт Анапа</t>
+  </si>
+  <si>
+    <t>город-курорт Геленджик</t>
   </si>
 </sst>
 </file>
@@ -8060,10 +8072,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:AP46"/>
+  <dimension ref="C4:AP52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8222,7 +8234,7 @@
       <c r="H5" s="7">
         <v>0.15749543280699099</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>24720.091919999999</v>
       </c>
       <c r="J5" s="7">
@@ -8265,57 +8277,59 @@
         <v>153.74505778284589</v>
       </c>
       <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
+      <c r="Y5" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="Z5" s="1">
-        <v>3578</v>
+        <v>1763</v>
       </c>
       <c r="AA5" s="1">
-        <v>47423</v>
+        <v>212839</v>
       </c>
       <c r="AB5" s="1">
-        <v>16239</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>37980</v>
+        <v>28526</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>23354.08466</v>
       </c>
       <c r="AD5" s="1">
-        <v>25765</v>
+        <v>141345.60000000001</v>
       </c>
       <c r="AE5" s="1">
-        <v>1125</v>
+        <v>24750</v>
       </c>
       <c r="AF5" s="1">
-        <v>2514578</v>
+        <v>21587685.325390004</v>
       </c>
       <c r="AG5" s="1">
-        <v>38.1</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="AH5" s="1">
-        <v>175</v>
+        <v>471</v>
       </c>
       <c r="AI5" s="1">
-        <v>53</v>
+        <v>284</v>
       </c>
       <c r="AJ5" s="1">
-        <v>569.79999999999995</v>
+        <v>966.6</v>
       </c>
       <c r="AK5" s="1">
-        <v>16799</v>
+        <v>186537</v>
       </c>
       <c r="AL5" s="1">
-        <v>130765.6</v>
+        <v>88881.7</v>
       </c>
       <c r="AM5" s="1">
-        <v>6645414.4000000004</v>
+        <v>3512839.4188999999</v>
       </c>
       <c r="AN5" s="1">
         <v>42</v>
       </c>
       <c r="AO5" s="1">
-        <v>2690</v>
+        <v>8643</v>
       </c>
       <c r="AP5" s="1">
-        <v>41419617.100000001</v>
+        <v>41903256.314429998</v>
       </c>
     </row>
     <row r="6" spans="3:42" x14ac:dyDescent="0.25">
@@ -8337,7 +8351,7 @@
       <c r="H6" s="7">
         <v>0.11616275402153831</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>21819.183840000002</v>
       </c>
       <c r="J6" s="7">
@@ -8380,24 +8394,60 @@
         <v>33.696300743477607</v>
       </c>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
+      <c r="Y6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>-43</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>115048</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>18845</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>25688.450580000001</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>146435</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>28940</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>14223515.170820002</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>42.7</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>307</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>614</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>399.1</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>13359</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>6852.2</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>425668.60330000002</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>25</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>5790</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>12400307.79752</v>
+      </c>
     </row>
     <row r="7" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -8418,7 +8468,7 @@
       <c r="H7" s="7">
         <v>0.24330836613491227</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>25219.131849999998</v>
       </c>
       <c r="J7" s="7">
@@ -8464,64 +8514,21 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="24">
-        <f>AB5/$AA5</f>
-        <v>0.34242877928431353</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>37980</v>
-      </c>
-      <c r="AD7" s="24">
-        <f t="shared" ref="AC7:AP7" si="0">AD5/$AA5</f>
-        <v>0.54330177340109231</v>
-      </c>
-      <c r="AE7" s="24">
-        <f t="shared" si="0"/>
-        <v>2.3722666216814625E-2</v>
-      </c>
-      <c r="AF7" s="24">
-        <f t="shared" si="0"/>
-        <v>53.024439617906921</v>
-      </c>
-      <c r="AG7" s="1">
-        <v>38.1</v>
-      </c>
-      <c r="AH7" s="24">
-        <f t="shared" si="0"/>
-        <v>3.6901925226156085E-3</v>
-      </c>
-      <c r="AI7" s="24">
-        <f t="shared" si="0"/>
-        <v>1.1176011639921558E-3</v>
-      </c>
-      <c r="AJ7" s="24">
-        <f t="shared" si="0"/>
-        <v>1.201526685363642E-2</v>
-      </c>
-      <c r="AK7" s="24">
-        <f t="shared" si="0"/>
-        <v>0.35423739535668347</v>
-      </c>
-      <c r="AL7" s="24">
-        <f t="shared" si="0"/>
-        <v>2.7574299390591066</v>
-      </c>
-      <c r="AM7" s="24">
-        <f t="shared" si="0"/>
-        <v>140.13062016321194</v>
-      </c>
-      <c r="AN7" s="24">
-        <f t="shared" si="0"/>
-        <v>8.8564620542774602E-4</v>
-      </c>
-      <c r="AO7" s="24">
-        <f t="shared" si="0"/>
-        <v>5.6723530776205636E-2</v>
-      </c>
-      <c r="AP7" s="24">
-        <f t="shared" si="0"/>
-        <v>873.40777892583776</v>
-      </c>
+      <c r="AB7" s="24"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="24"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="24"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="24"/>
+      <c r="AI7" s="24"/>
+      <c r="AJ7" s="24"/>
+      <c r="AK7" s="24"/>
+      <c r="AL7" s="24"/>
+      <c r="AM7" s="24"/>
+      <c r="AN7" s="24"/>
+      <c r="AO7" s="24"/>
+      <c r="AP7" s="24"/>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -8542,7 +8549,7 @@
       <c r="H8" s="7">
         <v>0.11754642600352069</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>19539.2</v>
       </c>
       <c r="J8" s="7">
@@ -8589,17 +8596,64 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="13"/>
-      <c r="AK8" s="13"/>
-      <c r="AL8" s="13"/>
+      <c r="AB8" s="13">
+        <f>AB5/$AA5</f>
+        <v>0.13402618880938175</v>
+      </c>
+      <c r="AC8" s="13">
+        <v>23354.08466</v>
+      </c>
+      <c r="AD8" s="13">
+        <f t="shared" ref="AC8:AP8" si="0">AD5/$AA5</f>
+        <v>0.66409633572794458</v>
+      </c>
+      <c r="AE8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.11628507933226523</v>
+      </c>
+      <c r="AF8" s="13">
+        <f t="shared" si="0"/>
+        <v>101.42730103688706</v>
+      </c>
+      <c r="AG8" s="13">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="AH8" s="13">
+        <f t="shared" si="0"/>
+        <v>2.2129402975958352E-3</v>
+      </c>
+      <c r="AI8" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3343419204187201E-3</v>
+      </c>
+      <c r="AJ8" s="13">
+        <f t="shared" si="0"/>
+        <v>4.5414609164673766E-3</v>
+      </c>
+      <c r="AK8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.87642302397586913</v>
+      </c>
+      <c r="AL8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.41760062770450901</v>
+      </c>
+      <c r="AM8" s="13">
+        <f t="shared" si="0"/>
+        <v>16.504679212456363</v>
+      </c>
+      <c r="AN8" s="13">
+        <f t="shared" si="0"/>
+        <v>1.9733225583657132E-4</v>
+      </c>
+      <c r="AO8" s="13">
+        <f t="shared" si="0"/>
+        <v>4.0608159218940135E-2</v>
+      </c>
+      <c r="AP8" s="13">
+        <f t="shared" si="0"/>
+        <v>196.87771655772673</v>
+      </c>
     </row>
     <row r="9" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -8620,7 +8674,7 @@
       <c r="H9" s="7">
         <v>0.34242877928431353</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>37980</v>
       </c>
       <c r="J9" s="7">
@@ -8662,9 +8716,126 @@
       <c r="V9" s="7">
         <v>873.40777892583776</v>
       </c>
+      <c r="AB9" s="13">
+        <f>AB6/$AA6</f>
+        <v>0.16380119602252974</v>
+      </c>
+      <c r="AC9" s="13">
+        <v>25688.450580000001</v>
+      </c>
+      <c r="AD9" s="13">
+        <f t="shared" ref="AC9:AP9" si="1">AD6/$AA6</f>
+        <v>1.2728165635213129</v>
+      </c>
+      <c r="AE9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25154718030734996</v>
+      </c>
+      <c r="AF9" s="13">
+        <f t="shared" si="1"/>
+        <v>123.63113805385579</v>
+      </c>
+      <c r="AG9" s="13">
+        <v>42.7</v>
+      </c>
+      <c r="AH9" s="13">
+        <f t="shared" si="1"/>
+        <v>2.6684514289687781E-3</v>
+      </c>
+      <c r="AI9" s="13">
+        <f t="shared" si="1"/>
+        <v>5.3369028579375562E-3</v>
+      </c>
+      <c r="AJ9" s="13">
+        <f t="shared" si="1"/>
+        <v>3.4689868576594121E-3</v>
+      </c>
+      <c r="AK9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.11611675126903553</v>
+      </c>
+      <c r="AL9" s="13">
+        <f t="shared" si="1"/>
+        <v>5.9559488213615182E-2</v>
+      </c>
+      <c r="AM9" s="13">
+        <f t="shared" si="1"/>
+        <v>3.6999218004658925</v>
+      </c>
+      <c r="AN9" s="13">
+        <f t="shared" si="1"/>
+        <v>2.1730060496488423E-4</v>
+      </c>
+      <c r="AO9" s="13">
+        <f t="shared" si="1"/>
+        <v>5.0326820109867186E-2</v>
+      </c>
+      <c r="AP9" s="13">
+        <f t="shared" si="1"/>
+        <v>107.78377544607469</v>
+      </c>
     </row>
     <row r="10" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="V10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1763</v>
+      </c>
+      <c r="G10" s="1">
+        <v>212839</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.13402618880938175</v>
+      </c>
+      <c r="I10" s="6">
+        <v>23354.08466</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.66409633572794458</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.11628507933226523</v>
+      </c>
+      <c r="L10" s="5">
+        <v>101.42730103688706</v>
+      </c>
+      <c r="M10" s="5">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="N10" s="5">
+        <v>2.2129402975958352E-3</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1.3343419204187201E-3</v>
+      </c>
+      <c r="P10" s="5">
+        <v>4.5414609164673766E-3</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0.87642302397586913</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.41760062770450901</v>
+      </c>
+      <c r="S10" s="5">
+        <v>16.504679212456363</v>
+      </c>
+      <c r="T10" s="5">
+        <v>1.9733225583657132E-4</v>
+      </c>
+      <c r="U10" s="5">
+        <v>4.0608159218940135E-2</v>
+      </c>
+      <c r="V10" s="5">
+        <v>196.87771655772673</v>
+      </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -8681,6 +8852,68 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
+    </row>
+    <row r="11" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-43</v>
+      </c>
+      <c r="G11" s="1">
+        <v>115048</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.16380119602252974</v>
+      </c>
+      <c r="I11" s="6">
+        <v>25688.450580000001</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.2728165635213129</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.25154718030734996</v>
+      </c>
+      <c r="L11" s="5">
+        <v>123.63113805385579</v>
+      </c>
+      <c r="M11" s="5">
+        <v>42.7</v>
+      </c>
+      <c r="N11" s="5">
+        <v>2.6684514289687781E-3</v>
+      </c>
+      <c r="O11" s="5">
+        <v>5.3369028579375562E-3</v>
+      </c>
+      <c r="P11" s="5">
+        <v>3.4689868576594121E-3</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0.11611675126903553</v>
+      </c>
+      <c r="R11" s="5">
+        <v>5.9559488213615182E-2</v>
+      </c>
+      <c r="S11" s="5">
+        <v>3.6999218004658925</v>
+      </c>
+      <c r="T11" s="5">
+        <v>2.1730060496488423E-4</v>
+      </c>
+      <c r="U11" s="5">
+        <v>5.0326820109867186E-2</v>
+      </c>
+      <c r="V11" s="5">
+        <v>107.78377544607469</v>
+      </c>
     </row>
     <row r="12" spans="3:42" x14ac:dyDescent="0.25">
       <c r="W12" s="1"/>
@@ -9316,874 +9549,1122 @@
         <v>4.9160000000000002E-2</v>
       </c>
     </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>3703000</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G25" s="7">
+        <v>6.0760000000000002E-2</v>
+      </c>
+      <c r="H25" s="7">
+        <v>6.207E-2</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5.2670000000000002E-2</v>
+      </c>
+      <c r="J25" s="7">
+        <v>4.6539999999999998E-2</v>
+      </c>
+      <c r="K25" s="7">
+        <v>3.8420000000000003E-2</v>
+      </c>
+      <c r="L25" s="7">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="M25" s="7">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="N25" s="7">
+        <v>8.8440000000000005E-2</v>
+      </c>
+      <c r="O25" s="7">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="P25" s="7">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.1244</v>
+      </c>
+      <c r="R25" s="7">
+        <v>7.6050000000000006E-2</v>
+      </c>
+      <c r="S25" s="7">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="T25" s="7">
+        <v>7.6799999999999993E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>3703000</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G26" s="7">
+        <v>7.1840000000000001E-2</v>
+      </c>
+      <c r="H26" s="7">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="I26" s="7">
+        <v>6.4699999999999994E-2</v>
+      </c>
+      <c r="J26" s="7">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="K26" s="7">
+        <v>4.1320000000000003E-2</v>
+      </c>
+      <c r="L26" s="7">
+        <v>6.93E-2</v>
+      </c>
+      <c r="M26" s="7">
+        <v>8.9539999999999995E-2</v>
+      </c>
+      <c r="N26" s="7">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="O26" s="7">
+        <v>7.6539999999999997E-2</v>
+      </c>
+      <c r="P26" s="7">
+        <v>6.9800000000000001E-2</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0.11053</v>
+      </c>
+      <c r="R26" s="7">
+        <v>6.5100000000000005E-2</v>
+      </c>
+      <c r="S26" s="7">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="T26" s="7">
+        <v>5.9970000000000002E-2</v>
+      </c>
+    </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D27" s="3" t="s">
-        <v>43</v>
+      <c r="C27" s="1">
+        <v>3708000</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G27" s="7">
+        <v>5.774E-2</v>
+      </c>
+      <c r="H27" s="7">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="I27" s="7">
+        <v>5.1479999999999998E-2</v>
+      </c>
+      <c r="J27" s="7">
+        <v>4.2569999999999997E-2</v>
+      </c>
+      <c r="K27" s="7">
+        <v>3.5430000000000003E-2</v>
+      </c>
+      <c r="L27" s="7">
+        <v>4.437E-2</v>
+      </c>
+      <c r="M27" s="7">
+        <v>8.0140000000000003E-2</v>
+      </c>
+      <c r="N27" s="7">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="O27" s="7">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="P27" s="7">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="R27" s="7">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="S27" s="7">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="T27" s="7">
+        <v>7.9039999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>3708000</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G28" s="7">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="H28" s="7">
+        <v>7.2749999999999995E-2</v>
+      </c>
+      <c r="I28" s="7">
+        <v>6.1830000000000003E-2</v>
+      </c>
+      <c r="J28" s="7">
+        <v>5.0659999999999997E-2</v>
+      </c>
+      <c r="K28" s="7">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="L28" s="7">
+        <v>5.3220000000000003E-2</v>
+      </c>
+      <c r="M28" s="7">
+        <v>8.0750000000000002E-2</v>
+      </c>
+      <c r="N28" s="7">
+        <v>9.1740000000000002E-2</v>
+      </c>
+      <c r="O28" s="7">
+        <v>8.5629999999999998E-2</v>
+      </c>
+      <c r="P28" s="7">
+        <v>7.1349999999999997E-2</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="R28" s="7">
+        <v>6.8900000000000003E-2</v>
+      </c>
+      <c r="S28" s="7">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="T28" s="7">
+        <v>6.2799999999999995E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="1">
         <v>0</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G33" s="7">
         <f>AVERAGE(G15,G17,G19,G21)</f>
         <v>5.7967500000000005E-2</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H33" s="7">
         <f>AVERAGE(H15,H17,H19,H21)</f>
         <v>6.6512500000000002E-2</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I33" s="7">
         <f>AVERAGE(I15,I17,I19,I21)</f>
         <v>6.3997499999999999E-2</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J33" s="7">
         <f>AVERAGE(J15,J17,J19,J21)</f>
         <v>5.0817500000000002E-2</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K33" s="7">
         <f>AVERAGE(K15,K17,K19,K21)</f>
         <v>5.4057499999999994E-2</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L33" s="7">
         <f>AVERAGE(L15,L17,L19,L21)</f>
         <v>5.3877500000000002E-2</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M33" s="7">
         <f>AVERAGE(M15,M17,M19,M21)</f>
         <v>7.4115E-2</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N33" s="7">
         <f>AVERAGE(N15,N17,N19,N21)</f>
         <v>7.55025E-2</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O33" s="7">
         <f>AVERAGE(O15,O17,O19,O21)</f>
         <v>7.1264999999999995E-2</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P33" s="7">
         <f>AVERAGE(P15,P17,P19,P21)</f>
         <v>7.0682499999999995E-2</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q33" s="7">
         <f>AVERAGE(Q15,Q17,Q19,Q21)</f>
         <v>0.1299525</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R33" s="7">
         <f>AVERAGE(R15,R17,R19,R21)</f>
         <v>8.3820000000000006E-2</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S33" s="7">
         <f>AVERAGE(S15,S17,S19,S21)</f>
         <v>8.3925E-2</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T33" s="7">
         <f>AVERAGE(T15,T17,T19,T21)</f>
         <v>6.3485E-2</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D28" s="3" t="s">
+    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F34" s="1">
         <v>0</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G34" s="7">
         <f>AVERAGE(G16,G18,G20,G22)</f>
         <v>6.2570000000000001E-2</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H34" s="7">
         <f>AVERAGE(H16,H18,H20,H22)</f>
         <v>7.2730000000000017E-2</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I34" s="7">
         <f>AVERAGE(I16,I18,I20,I22)</f>
         <v>7.0974999999999996E-2</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J34" s="7">
         <f>AVERAGE(J16,J18,J20,J22)</f>
         <v>5.8692499999999995E-2</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K34" s="7">
         <f>AVERAGE(K16,K18,K20,K22)</f>
         <v>5.7327500000000003E-2</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L34" s="7">
         <f>AVERAGE(L16,L18,L20,L22)</f>
         <v>6.9550000000000001E-2</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M34" s="7">
         <f>AVERAGE(M16,M18,M20,M22)</f>
         <v>8.2485000000000003E-2</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N34" s="7">
         <f>AVERAGE(N16,N18,N20,N22)</f>
         <v>7.9822500000000005E-2</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O34" s="7">
         <f>AVERAGE(O16,O18,O20,O22)</f>
         <v>7.041E-2</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P34" s="7">
         <f>AVERAGE(P16,P18,P20,P22)</f>
         <v>7.0554999999999993E-2</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q34" s="7">
         <f>AVERAGE(Q16,Q18,Q20,Q22)</f>
         <v>0.11919250000000001</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R34" s="7">
         <f>AVERAGE(R16,R18,R20,R22)</f>
         <v>7.4567499999999995E-2</v>
       </c>
-      <c r="S28" s="7">
+      <c r="S34" s="7">
         <f>AVERAGE(S16,S18,S20,S22)</f>
         <v>6.8182499999999993E-2</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T34" s="7">
         <f>AVERAGE(T16,T18,T20,T22)</f>
         <v>4.3022500000000005E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
+    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="Q39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="R39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S33" s="2" t="s">
+      <c r="S39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T33" s="2" t="s">
+      <c r="T39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="U39" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V33" s="2" t="s">
+      <c r="V39" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D34" s="1" t="s">
+    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E40" s="1">
         <v>2015</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F40" s="1">
         <v>-508</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G40" s="1">
         <v>89673</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H40" s="1">
         <v>0.17097677115742749</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I40" s="1">
         <v>20274.726180000001</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J40" s="1">
         <v>0.63144982324668508</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K40" s="1">
         <v>1.8846252495176911E-2</v>
       </c>
-      <c r="L34" s="1">
+      <c r="L40" s="1">
         <v>23.73828289719313</v>
       </c>
-      <c r="M34" s="1">
+      <c r="M40" s="1">
         <v>25.6</v>
       </c>
-      <c r="N34" s="1">
+      <c r="N40" s="1">
         <v>5.8769083224604586E-3</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O40" s="1">
         <v>2.9663332329686628E-3</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P40" s="1">
         <v>8.227671651444687E-3</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="Q40" s="1">
         <v>1.0814961025057701</v>
       </c>
-      <c r="R34" s="1">
+      <c r="R40" s="1">
         <v>0.67026351298607134</v>
       </c>
-      <c r="S34" s="1">
+      <c r="S40" s="1">
         <v>25.881326426014489</v>
       </c>
-      <c r="T34" s="1">
+      <c r="T40" s="1">
         <v>4.9067166259632105E-4</v>
       </c>
-      <c r="U34" s="1">
+      <c r="U40" s="1">
         <v>5.6929064489868737E-2</v>
       </c>
-      <c r="V34" s="1">
+      <c r="V40" s="1">
         <v>119.345016326319</v>
-      </c>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F35" s="1">
-        <v>-583</v>
-      </c>
-      <c r="G35" s="1">
-        <v>88968</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0.1689259059437101</v>
-      </c>
-      <c r="I35" s="1">
-        <v>21016.71081</v>
-      </c>
-      <c r="J35" s="1">
-        <v>0.63645580433414262</v>
-      </c>
-      <c r="K35" s="1">
-        <v>1.899559392140994E-2</v>
-      </c>
-      <c r="L35" s="1">
-        <v>23.527577473473599</v>
-      </c>
-      <c r="M35" s="1">
-        <v>26.6</v>
-      </c>
-      <c r="N35" s="1">
-        <v>5.9234781044869714E-3</v>
-      </c>
-      <c r="O35" s="1">
-        <v>3.0572790216706999E-3</v>
-      </c>
-      <c r="P35" s="1">
-        <v>8.4412372988040517E-3</v>
-      </c>
-      <c r="Q35" s="1">
-        <v>1.082479093606689</v>
-      </c>
-      <c r="R35" s="1">
-        <v>0.61311033180469354</v>
-      </c>
-      <c r="S35" s="1">
-        <v>24.770910734196551</v>
-      </c>
-      <c r="T35" s="1">
-        <v>4.9455984174084965E-4</v>
-      </c>
-      <c r="U35" s="1">
-        <v>5.7874741480082717E-2</v>
-      </c>
-      <c r="V35" s="1">
-        <v>143.61354485994971</v>
-      </c>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="1">
-        <v>2017</v>
-      </c>
-      <c r="F36" s="1">
-        <v>-507</v>
-      </c>
-      <c r="G36" s="1">
-        <v>88092</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.1657471734096172</v>
-      </c>
-      <c r="I36" s="1">
-        <v>22275.830239999999</v>
-      </c>
-      <c r="J36" s="1">
-        <v>0.67765063796939562</v>
-      </c>
-      <c r="K36" s="1">
-        <v>1.9740725605049251E-2</v>
-      </c>
-      <c r="L36" s="1">
-        <v>26.707001895631841</v>
-      </c>
-      <c r="M36" s="1">
-        <v>27.4</v>
-      </c>
-      <c r="N36" s="1">
-        <v>5.9823820551241514E-3</v>
-      </c>
-      <c r="O36" s="1">
-        <v>3.0536257548926002E-3</v>
-      </c>
-      <c r="P36" s="1">
-        <v>8.7851337238341615E-3</v>
-      </c>
-      <c r="Q36" s="1">
-        <v>1.0234073468646401</v>
-      </c>
-      <c r="R36" s="1">
-        <v>0.61994051673250683</v>
-      </c>
-      <c r="S36" s="1">
-        <v>21.178866225082849</v>
-      </c>
-      <c r="T36" s="1">
-        <v>4.9947781864414359E-4</v>
-      </c>
-      <c r="U36" s="1">
-        <v>5.87113472278981E-2</v>
-      </c>
-      <c r="V36" s="1">
-        <v>142.04406721007581</v>
-      </c>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F37" s="1">
-        <v>-711</v>
-      </c>
-      <c r="G37" s="1">
-        <v>87282</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.16122453655965721</v>
-      </c>
-      <c r="I37" s="1">
-        <v>23989.908439999999</v>
-      </c>
-      <c r="J37" s="1">
-        <v>0.68737654957494088</v>
-      </c>
-      <c r="K37" s="1">
-        <v>1.875529891615681E-2</v>
-      </c>
-      <c r="L37" s="1">
-        <v>29.351305275772781</v>
-      </c>
-      <c r="M37" s="1">
-        <v>28.1</v>
-      </c>
-      <c r="N37" s="1">
-        <v>6.3586993881899652E-3</v>
-      </c>
-      <c r="O37" s="1">
-        <v>3.0819642079695569E-3</v>
-      </c>
-      <c r="P37" s="1">
-        <v>9.3810865928828282E-3</v>
-      </c>
-      <c r="Q37" s="1">
-        <v>0.98409752297151609</v>
-      </c>
-      <c r="R37" s="1">
-        <v>0.71611913109232095</v>
-      </c>
-      <c r="S37" s="1">
-        <v>20.416691414037231</v>
-      </c>
-      <c r="T37" s="1">
-        <v>5.0411310464929633E-4</v>
-      </c>
-      <c r="U37" s="1">
-        <v>5.925620402832199E-2</v>
-      </c>
-      <c r="V37" s="1">
-        <v>145.038276238858</v>
-      </c>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="3">
-        <v>2020</v>
-      </c>
-      <c r="F38" s="1">
-        <v>-151.99999999999989</v>
-      </c>
-      <c r="G38" s="1">
-        <v>85939</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0.15749543280699099</v>
-      </c>
-      <c r="I38" s="1">
-        <v>24720.091919999999</v>
-      </c>
-      <c r="J38" s="1">
-        <v>0.81039690943576237</v>
-      </c>
-      <c r="K38" s="1">
-        <v>1.8396769801836171E-2</v>
-      </c>
-      <c r="L38" s="1">
-        <v>32.194688077822633</v>
-      </c>
-      <c r="M38" s="1">
-        <v>28.7</v>
-      </c>
-      <c r="N38" s="1">
-        <v>6.539522219248496E-3</v>
-      </c>
-      <c r="O38" s="1">
-        <v>2.5715914776760149E-3</v>
-      </c>
-      <c r="P38" s="1">
-        <v>1.0555161219004169E-2</v>
-      </c>
-      <c r="Q38" s="1">
-        <v>1.1495013905211819</v>
-      </c>
-      <c r="R38" s="1">
-        <v>0.66520904362396571</v>
-      </c>
-      <c r="S38" s="1">
-        <v>22.581482595794672</v>
-      </c>
-      <c r="T38" s="1">
-        <v>7.4471427407812321E-4</v>
-      </c>
-      <c r="U38" s="1">
-        <v>6.0112405310743661E-2</v>
-      </c>
-      <c r="V38" s="1">
-        <v>153.74505778284589</v>
       </c>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>16</v>
+      <c r="D41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-583</v>
+      </c>
+      <c r="G41" s="1">
+        <v>88968</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.1689259059437101</v>
+      </c>
+      <c r="I41" s="1">
+        <v>21016.71081</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.63645580433414262</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1.899559392140994E-2</v>
+      </c>
+      <c r="L41" s="1">
+        <v>23.527577473473599</v>
+      </c>
+      <c r="M41" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="N41" s="1">
+        <v>5.9234781044869714E-3</v>
+      </c>
+      <c r="O41" s="1">
+        <v>3.0572790216706999E-3</v>
+      </c>
+      <c r="P41" s="1">
+        <v>8.4412372988040517E-3</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>1.082479093606689</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0.61311033180469354</v>
+      </c>
+      <c r="S41" s="1">
+        <v>24.770910734196551</v>
+      </c>
+      <c r="T41" s="1">
+        <v>4.9455984174084965E-4</v>
+      </c>
+      <c r="U41" s="1">
+        <v>5.7874741480082717E-2</v>
+      </c>
+      <c r="V41" s="1">
+        <v>143.61354485994971</v>
       </c>
     </row>
     <row r="42" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="23" t="s">
-        <v>70</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="F42" s="1">
-        <v>-163</v>
+        <v>-507</v>
       </c>
       <c r="G42" s="1">
-        <v>44795</v>
+        <v>88092</v>
       </c>
       <c r="H42" s="1">
-        <v>0.1195669159504409</v>
+        <v>0.1657471734096172</v>
       </c>
       <c r="I42" s="1">
-        <v>19632.524519999999</v>
+        <v>22275.830239999999</v>
       </c>
       <c r="J42" s="1">
-        <v>0.26123004799642802</v>
+        <v>0.67765063796939562</v>
       </c>
       <c r="K42" s="1">
-        <v>3.0717714030583751E-2</v>
+        <v>1.9740725605049251E-2</v>
       </c>
       <c r="L42" s="1">
-        <v>6.8428243203482468</v>
+        <v>26.707001895631841</v>
       </c>
       <c r="M42" s="1">
-        <v>25.4</v>
+        <v>27.4</v>
       </c>
       <c r="N42" s="1">
-        <v>3.415559772295994E-3</v>
+        <v>5.9823820551241514E-3</v>
       </c>
       <c r="O42" s="1">
-        <v>2.2993637682777002E-3</v>
+        <v>3.0536257548926002E-3</v>
       </c>
       <c r="P42" s="1">
-        <v>1.320683111954458E-2</v>
+        <v>8.7851337238341615E-3</v>
       </c>
       <c r="Q42" s="1">
-        <v>3.216117870298024</v>
+        <v>1.0234073468646401</v>
       </c>
       <c r="R42" s="1">
-        <v>0.54021386315436981</v>
+        <v>0.61994051673250683</v>
       </c>
       <c r="S42" s="1">
-        <v>65.877446219444096</v>
+        <v>21.178866225082849</v>
       </c>
       <c r="T42" s="1">
-        <v>1.5626744056256249E-3</v>
+        <v>4.9947781864414359E-4</v>
       </c>
       <c r="U42" s="1">
-        <v>4.6790936488447371E-2</v>
+        <v>5.87113472278981E-2</v>
       </c>
       <c r="V42" s="1">
-        <v>36.086993072441103</v>
+        <v>142.04406721007581</v>
       </c>
     </row>
     <row r="43" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="23" t="s">
-        <v>70</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E43" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="F43" s="1">
-        <v>-100</v>
+        <v>-711</v>
       </c>
       <c r="G43" s="1">
-        <v>44888</v>
+        <v>87282</v>
       </c>
       <c r="H43" s="1">
-        <v>0.1251559436820531</v>
+        <v>0.16122453655965721</v>
       </c>
       <c r="I43" s="1">
-        <v>18340.544890000001</v>
+        <v>23989.908439999999</v>
       </c>
       <c r="J43" s="1">
-        <v>0.37225984672963802</v>
+        <v>0.68737654957494088</v>
       </c>
       <c r="K43" s="1">
-        <v>3.412938870076633E-2</v>
+        <v>1.875529891615681E-2</v>
       </c>
       <c r="L43" s="1">
-        <v>8.4181796671716178</v>
+        <v>29.351305275772781</v>
       </c>
       <c r="M43" s="1">
-        <v>27.3</v>
+        <v>28.1</v>
       </c>
       <c r="N43" s="1">
-        <v>3.2970949919800181E-3</v>
+        <v>6.3586993881899652E-3</v>
       </c>
       <c r="O43" s="1">
-        <v>2.31687756193191E-3</v>
+        <v>3.0819642079695569E-3</v>
       </c>
       <c r="P43" s="1">
-        <v>1.3460167528069861E-2</v>
+        <v>9.3810865928828282E-3</v>
       </c>
       <c r="Q43" s="1">
-        <v>3.237123507396185</v>
+        <v>0.98409752297151609</v>
       </c>
       <c r="R43" s="1">
-        <v>0.44668731063981459</v>
+        <v>0.71611913109232095</v>
       </c>
       <c r="S43" s="1">
-        <v>65.029295230351053</v>
+        <v>20.416691414037231</v>
       </c>
       <c r="T43" s="1">
-        <v>1.559436820531096E-3</v>
+        <v>5.0411310464929633E-4</v>
       </c>
       <c r="U43" s="1">
-        <v>4.7696489039386912E-2</v>
+        <v>5.925620402832199E-2</v>
       </c>
       <c r="V43" s="1">
-        <v>36.327307061575482</v>
+        <v>145.038276238858</v>
       </c>
     </row>
     <row r="44" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-151.99999999999989</v>
+      </c>
+      <c r="G44" s="1">
+        <v>85939</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.15749543280699099</v>
+      </c>
+      <c r="I44" s="1">
+        <v>24720.091919999999</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.81039690943576237</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1.8396769801836171E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <v>32.194688077822633</v>
+      </c>
+      <c r="M44" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="N44" s="1">
+        <v>6.539522219248496E-3</v>
+      </c>
+      <c r="O44" s="1">
+        <v>2.5715914776760149E-3</v>
+      </c>
+      <c r="P44" s="1">
+        <v>1.0555161219004169E-2</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>1.1495013905211819</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0.66520904362396571</v>
+      </c>
+      <c r="S44" s="1">
+        <v>22.581482595794672</v>
+      </c>
+      <c r="T44" s="1">
+        <v>7.4471427407812321E-4</v>
+      </c>
+      <c r="U44" s="1">
+        <v>6.0112405310743661E-2</v>
+      </c>
+      <c r="V44" s="1">
+        <v>153.74505778284589</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C48" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E48" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F48" s="1">
+        <v>-163</v>
+      </c>
+      <c r="G48" s="1">
+        <v>44795</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.1195669159504409</v>
+      </c>
+      <c r="I48" s="1">
+        <v>19632.524519999999</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.26123004799642802</v>
+      </c>
+      <c r="K48" s="1">
+        <v>3.0717714030583751E-2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>6.8428243203482468</v>
+      </c>
+      <c r="M48" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="N48" s="1">
+        <v>3.415559772295994E-3</v>
+      </c>
+      <c r="O48" s="1">
+        <v>2.2993637682777002E-3</v>
+      </c>
+      <c r="P48" s="1">
+        <v>1.320683111954458E-2</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>3.216117870298024</v>
+      </c>
+      <c r="R48" s="1">
+        <v>0.54021386315436981</v>
+      </c>
+      <c r="S48" s="1">
+        <v>65.877446219444096</v>
+      </c>
+      <c r="T48" s="1">
+        <v>1.5626744056256249E-3</v>
+      </c>
+      <c r="U48" s="1">
+        <v>4.6790936488447371E-2</v>
+      </c>
+      <c r="V48" s="1">
+        <v>36.086993072441103</v>
+      </c>
+    </row>
+    <row r="49" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C49" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F49" s="1">
+        <v>-100</v>
+      </c>
+      <c r="G49" s="1">
+        <v>44888</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.1251559436820531</v>
+      </c>
+      <c r="I49" s="1">
+        <v>18340.544890000001</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.37225984672963802</v>
+      </c>
+      <c r="K49" s="1">
+        <v>3.412938870076633E-2</v>
+      </c>
+      <c r="L49" s="1">
+        <v>8.4181796671716178</v>
+      </c>
+      <c r="M49" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="N49" s="1">
+        <v>3.2970949919800181E-3</v>
+      </c>
+      <c r="O49" s="1">
+        <v>2.31687756193191E-3</v>
+      </c>
+      <c r="P49" s="1">
+        <v>1.3460167528069861E-2</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>3.237123507396185</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0.44668731063981459</v>
+      </c>
+      <c r="S49" s="1">
+        <v>65.029295230351053</v>
+      </c>
+      <c r="T49" s="1">
+        <v>1.559436820531096E-3</v>
+      </c>
+      <c r="U49" s="1">
+        <v>4.7696489039386912E-2</v>
+      </c>
+      <c r="V49" s="1">
+        <v>36.327307061575482</v>
+      </c>
+    </row>
+    <row r="50" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C50" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="1">
         <v>2017</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F50" s="1">
         <v>-179</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G50" s="1">
         <v>44962</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H50" s="1">
         <v>0.1264401049775366</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I50" s="1">
         <v>19591.68519</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J50" s="1">
         <v>0.37287042391352693</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K50" s="1">
         <v>3.0603620835372079E-2</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L50" s="1">
         <v>22.083162368444469</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M50" s="1">
         <v>28.1</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N50" s="1">
         <v>3.6475245763088601E-3</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O50" s="1">
         <v>2.3130643654641599E-3</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P50" s="1">
         <v>1.3724923268537871E-2</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="Q50" s="1">
         <v>3.2863529202437611</v>
       </c>
-      <c r="R44" s="1">
+      <c r="R50" s="1">
         <v>0.48064810284240023</v>
       </c>
-      <c r="S44" s="1">
+      <c r="S50" s="1">
         <v>62.958639059650331</v>
       </c>
-      <c r="T44" s="1">
+      <c r="T50" s="1">
         <v>1.5568702459854949E-3</v>
       </c>
-      <c r="U44" s="1">
+      <c r="U50" s="1">
         <v>4.7617988523642192E-2</v>
       </c>
-      <c r="V44" s="1">
+      <c r="V50" s="1">
         <v>38.445424051198778</v>
       </c>
     </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="23" t="s">
+    <row r="51" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C51" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E51" s="1">
         <v>2018</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F51" s="1">
         <v>-56.99999999999995</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G51" s="1">
         <v>44933.999999999993</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H51" s="1">
         <v>0.1135665642942983</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I51" s="1">
         <v>20641.733639999999</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J51" s="1">
         <v>0.37868206703164631</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K51" s="1">
         <v>3.4984644144745607E-2</v>
       </c>
-      <c r="L45" s="1">
+      <c r="L51" s="1">
         <v>23.389734217296478</v>
       </c>
-      <c r="M45" s="1">
+      <c r="M51" s="1">
         <v>28.8</v>
       </c>
-      <c r="N45" s="1">
+      <c r="N51" s="1">
         <v>3.7165620688120122E-3</v>
       </c>
-      <c r="O45" s="1">
+      <c r="O51" s="1">
         <v>2.2699959941247069E-3</v>
       </c>
-      <c r="P45" s="1">
+      <c r="P51" s="1">
         <v>1.374237770952952E-2</v>
       </c>
-      <c r="Q45" s="1">
+      <c r="Q51" s="1">
         <v>2.790626251836025</v>
       </c>
-      <c r="R45" s="1">
+      <c r="R51" s="1">
         <v>0.49644456313704521</v>
       </c>
-      <c r="S45" s="1">
+      <c r="S51" s="1">
         <v>59.326706022165851</v>
       </c>
-      <c r="T45" s="1">
+      <c r="T51" s="1">
         <v>1.491075800062311E-3</v>
       </c>
-      <c r="U45" s="1">
+      <c r="U51" s="1">
         <v>4.775893532736903E-2</v>
       </c>
-      <c r="V45" s="1">
+      <c r="V51" s="1">
         <v>34.524197758490182</v>
       </c>
     </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C46" s="3" t="s">
+    <row r="52" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E52" s="3">
         <v>2020</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F52" s="1">
         <v>-449.99999999999989</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G52" s="1">
         <v>44386</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H52" s="1">
         <v>0.11616275402153831</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I52" s="1">
         <v>21819.183840000002</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J52" s="1">
         <v>0.43312530978236369</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K52" s="1">
         <v>3.4515387734871332E-2</v>
       </c>
-      <c r="L46" s="1">
+      <c r="L52" s="1">
         <v>23.330135132699489</v>
       </c>
-      <c r="M46" s="1">
+      <c r="M52" s="1">
         <v>29.9</v>
       </c>
-      <c r="N46" s="1">
+      <c r="N52" s="1">
         <v>3.807506871536046E-3</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O52" s="1">
         <v>2.343081151714495E-3</v>
       </c>
-      <c r="P46" s="1">
+      <c r="P52" s="1">
         <v>1.4168882079935099E-2</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="Q52" s="1">
         <v>2.863042400756993</v>
       </c>
-      <c r="R46" s="1">
+      <c r="R52" s="1">
         <v>0.49934596494390132</v>
       </c>
-      <c r="S46" s="1">
+      <c r="S52" s="1">
         <v>56.510477592033467</v>
       </c>
-      <c r="T46" s="1">
+      <c r="T52" s="1">
         <v>1.622133105033115E-3</v>
       </c>
-      <c r="U46" s="1">
+      <c r="U52" s="1">
         <v>4.9587707835804067E-2</v>
       </c>
-      <c r="V46" s="1">
+      <c r="V52" s="1">
         <v>33.696300743477607</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I34:I38">
+  <conditionalFormatting sqref="I40:I44">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L40:L44">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q40:Q44">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -10195,7 +10676,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L34:L38">
+  <conditionalFormatting sqref="R40:R44">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -10207,7 +10688,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q34:Q38">
+  <conditionalFormatting sqref="S40:S44">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -10219,7 +10700,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R34:R38">
+  <conditionalFormatting sqref="V40:V44">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -10231,7 +10712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S34:S38">
+  <conditionalFormatting sqref="I48:I52">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -10243,7 +10724,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V34:V38">
+  <conditionalFormatting sqref="L48:L52">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -10255,7 +10736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:I46">
+  <conditionalFormatting sqref="Q48:Q52">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -10267,7 +10748,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L42:L46">
+  <conditionalFormatting sqref="R48:R52">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -10279,7 +10760,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q42:Q46">
+  <conditionalFormatting sqref="S48:S52">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -10291,7 +10772,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R42:R46">
+  <conditionalFormatting sqref="V48:V52">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -10303,7 +10784,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S42:S46">
+  <conditionalFormatting sqref="G15:T15">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -10315,7 +10796,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V42:V46">
+  <conditionalFormatting sqref="G16:T16">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -10327,7 +10808,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:T15">
+  <conditionalFormatting sqref="G17:T17">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -10339,7 +10820,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:T16">
+  <conditionalFormatting sqref="G18:T18">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -10351,7 +10832,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:T17">
+  <conditionalFormatting sqref="G19:T20">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -10363,7 +10844,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18:T18">
+  <conditionalFormatting sqref="G21:T22">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -10375,7 +10856,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:T20">
+  <conditionalFormatting sqref="G23:T24">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -10387,7 +10868,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:T22">
+  <conditionalFormatting sqref="G25:T26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -10399,7 +10880,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23:T24">
+  <conditionalFormatting sqref="G27:T28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Protest in Angarsk 2020
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/soc-conflicts analysis.xlsx
+++ b/migforecasting/social conflicts/soc-conflicts analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="75">
   <si>
     <t>saldo</t>
   </si>
@@ -241,16 +241,13 @@
     <t>Лаишевский МР</t>
   </si>
   <si>
-    <t>Анапа</t>
-  </si>
-  <si>
-    <t>Геленджик</t>
-  </si>
-  <si>
     <t>город-курорт Анапа</t>
   </si>
   <si>
     <t>город-курорт Геленджик</t>
+  </si>
+  <si>
+    <t>Ангарский</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,7 +435,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -8072,10 +8068,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:AP52"/>
+  <dimension ref="C4:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8278,58 +8274,58 @@
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="1">
-        <v>1763</v>
+        <v>-194</v>
       </c>
       <c r="AA5" s="1">
-        <v>212839</v>
+        <v>236912</v>
       </c>
       <c r="AB5" s="1">
-        <v>28526</v>
-      </c>
-      <c r="AC5" s="7">
-        <v>23354.08466</v>
+        <v>53549</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>34942.071599999996</v>
       </c>
       <c r="AD5" s="1">
-        <v>141345.60000000001</v>
+        <v>235660</v>
       </c>
       <c r="AE5" s="1">
-        <v>24750</v>
+        <v>8148</v>
       </c>
       <c r="AF5" s="1">
-        <v>21587685.325390004</v>
+        <v>11652446.762639999</v>
       </c>
       <c r="AG5" s="1">
-        <v>38.700000000000003</v>
+        <v>23.7</v>
       </c>
       <c r="AH5" s="1">
-        <v>471</v>
+        <v>404</v>
       </c>
       <c r="AI5" s="1">
-        <v>284</v>
+        <v>916</v>
       </c>
       <c r="AJ5" s="1">
-        <v>966.6</v>
+        <v>472.3</v>
       </c>
       <c r="AK5" s="1">
-        <v>186537</v>
+        <v>8869</v>
       </c>
       <c r="AL5" s="1">
-        <v>88881.7</v>
+        <v>69835</v>
       </c>
       <c r="AM5" s="1">
-        <v>3512839.4188999999</v>
+        <v>1877904.9180000001</v>
       </c>
       <c r="AN5" s="1">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="AO5" s="1">
-        <v>8643</v>
+        <v>13689</v>
       </c>
       <c r="AP5" s="1">
-        <v>41903256.314429998</v>
+        <v>67922741.907359987</v>
       </c>
     </row>
     <row r="6" spans="3:42" x14ac:dyDescent="0.25">
@@ -8394,60 +8390,24 @@
         <v>33.696300743477607</v>
       </c>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>-43</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>115048</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>18845</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>25688.450580000001</v>
-      </c>
-      <c r="AD6" s="1">
-        <v>146435</v>
-      </c>
-      <c r="AE6" s="1">
-        <v>28940</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>14223515.170820002</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>42.7</v>
-      </c>
-      <c r="AH6" s="1">
-        <v>307</v>
-      </c>
-      <c r="AI6" s="1">
-        <v>614</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>399.1</v>
-      </c>
-      <c r="AK6" s="1">
-        <v>13359</v>
-      </c>
-      <c r="AL6" s="1">
-        <v>6852.2</v>
-      </c>
-      <c r="AM6" s="1">
-        <v>425668.60330000002</v>
-      </c>
-      <c r="AN6" s="1">
-        <v>25</v>
-      </c>
-      <c r="AO6" s="1">
-        <v>5790</v>
-      </c>
-      <c r="AP6" s="1">
-        <v>12400307.79752</v>
-      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
     </row>
     <row r="7" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -8514,21 +8474,64 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="24"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="24"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="24"/>
-      <c r="AK7" s="24"/>
-      <c r="AL7" s="24"/>
-      <c r="AM7" s="24"/>
-      <c r="AN7" s="24"/>
-      <c r="AO7" s="24"/>
-      <c r="AP7" s="24"/>
+      <c r="AB7" s="1">
+        <f>AB5/$AA5</f>
+        <v>0.22602907408658068</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>34942.071599999996</v>
+      </c>
+      <c r="AD7" s="1">
+        <f t="shared" ref="AC7:AP7" si="0">AD5/$AA5</f>
+        <v>0.99471533734044704</v>
+      </c>
+      <c r="AE7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4392517052745326E-2</v>
+      </c>
+      <c r="AF7" s="1">
+        <f t="shared" si="0"/>
+        <v>49.184704711622878</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="AH7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7052745323157966E-3</v>
+      </c>
+      <c r="AI7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8664145336665093E-3</v>
+      </c>
+      <c r="AJ7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9935672317147298E-3</v>
+      </c>
+      <c r="AK7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7435841156209904E-2</v>
+      </c>
+      <c r="AL7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29477189842641993</v>
+      </c>
+      <c r="AM7" s="1">
+        <f t="shared" si="0"/>
+        <v>7.9265926504356052</v>
+      </c>
+      <c r="AN7" s="1">
+        <f t="shared" si="0"/>
+        <v>7.5977578172485983E-5</v>
+      </c>
+      <c r="AO7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.778094820017559E-2</v>
+      </c>
+      <c r="AP7" s="1">
+        <f t="shared" si="0"/>
+        <v>286.70030183089074</v>
+      </c>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -8596,64 +8599,21 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
-      <c r="AB8" s="13">
-        <f>AB5/$AA5</f>
-        <v>0.13402618880938175</v>
-      </c>
-      <c r="AC8" s="13">
-        <v>23354.08466</v>
-      </c>
-      <c r="AD8" s="13">
-        <f t="shared" ref="AC8:AP8" si="0">AD5/$AA5</f>
-        <v>0.66409633572794458</v>
-      </c>
-      <c r="AE8" s="13">
-        <f t="shared" si="0"/>
-        <v>0.11628507933226523</v>
-      </c>
-      <c r="AF8" s="13">
-        <f t="shared" si="0"/>
-        <v>101.42730103688706</v>
-      </c>
-      <c r="AG8" s="13">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="AH8" s="13">
-        <f t="shared" si="0"/>
-        <v>2.2129402975958352E-3</v>
-      </c>
-      <c r="AI8" s="13">
-        <f t="shared" si="0"/>
-        <v>1.3343419204187201E-3</v>
-      </c>
-      <c r="AJ8" s="13">
-        <f t="shared" si="0"/>
-        <v>4.5414609164673766E-3</v>
-      </c>
-      <c r="AK8" s="13">
-        <f t="shared" si="0"/>
-        <v>0.87642302397586913</v>
-      </c>
-      <c r="AL8" s="13">
-        <f t="shared" si="0"/>
-        <v>0.41760062770450901</v>
-      </c>
-      <c r="AM8" s="13">
-        <f t="shared" si="0"/>
-        <v>16.504679212456363</v>
-      </c>
-      <c r="AN8" s="13">
-        <f t="shared" si="0"/>
-        <v>1.9733225583657132E-4</v>
-      </c>
-      <c r="AO8" s="13">
-        <f t="shared" si="0"/>
-        <v>4.0608159218940135E-2</v>
-      </c>
-      <c r="AP8" s="13">
-        <f t="shared" si="0"/>
-        <v>196.87771655772673</v>
-      </c>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
     </row>
     <row r="9" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -8716,71 +8676,28 @@
       <c r="V9" s="7">
         <v>873.40777892583776</v>
       </c>
-      <c r="AB9" s="13">
-        <f>AB6/$AA6</f>
-        <v>0.16380119602252974</v>
-      </c>
-      <c r="AC9" s="13">
-        <v>25688.450580000001</v>
-      </c>
-      <c r="AD9" s="13">
-        <f t="shared" ref="AC9:AP9" si="1">AD6/$AA6</f>
-        <v>1.2728165635213129</v>
-      </c>
-      <c r="AE9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.25154718030734996</v>
-      </c>
-      <c r="AF9" s="13">
-        <f t="shared" si="1"/>
-        <v>123.63113805385579</v>
-      </c>
-      <c r="AG9" s="13">
-        <v>42.7</v>
-      </c>
-      <c r="AH9" s="13">
-        <f t="shared" si="1"/>
-        <v>2.6684514289687781E-3</v>
-      </c>
-      <c r="AI9" s="13">
-        <f t="shared" si="1"/>
-        <v>5.3369028579375562E-3</v>
-      </c>
-      <c r="AJ9" s="13">
-        <f t="shared" si="1"/>
-        <v>3.4689868576594121E-3</v>
-      </c>
-      <c r="AK9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.11611675126903553</v>
-      </c>
-      <c r="AL9" s="13">
-        <f t="shared" si="1"/>
-        <v>5.9559488213615182E-2</v>
-      </c>
-      <c r="AM9" s="13">
-        <f t="shared" si="1"/>
-        <v>3.6999218004658925</v>
-      </c>
-      <c r="AN9" s="13">
-        <f t="shared" si="1"/>
-        <v>2.1730060496488423E-4</v>
-      </c>
-      <c r="AO9" s="13">
-        <f t="shared" si="1"/>
-        <v>5.0326820109867186E-2</v>
-      </c>
-      <c r="AP9" s="13">
-        <f t="shared" si="1"/>
-        <v>107.78377544607469</v>
-      </c>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
     </row>
     <row r="10" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1">
         <v>2021</v>
@@ -8858,7 +8775,7 @@
         <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="1">
         <v>2021</v>
@@ -8916,6 +8833,66 @@
       </c>
     </row>
     <row r="12" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-194</v>
+      </c>
+      <c r="G12" s="1">
+        <v>236912</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.22602907408658068</v>
+      </c>
+      <c r="I12" s="6">
+        <v>34942.071599999996</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.99471533734044704</v>
+      </c>
+      <c r="K12" s="5">
+        <v>3.4392517052745326E-2</v>
+      </c>
+      <c r="L12" s="5">
+        <v>49.184704711622878</v>
+      </c>
+      <c r="M12" s="5">
+        <v>23.7</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1.7052745323157966E-3</v>
+      </c>
+      <c r="O12" s="5">
+        <v>3.8664145336665093E-3</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1.9935672317147298E-3</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>3.7435841156209904E-2</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.29477189842641993</v>
+      </c>
+      <c r="S12" s="5">
+        <v>7.9265926504356052</v>
+      </c>
+      <c r="T12" s="5">
+        <v>7.5977578172485983E-5</v>
+      </c>
+      <c r="U12" s="5">
+        <v>5.778094820017559E-2</v>
+      </c>
+      <c r="V12" s="5">
+        <v>286.70030183089074</v>
+      </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -8933,116 +8910,60 @@
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
     </row>
-    <row r="14" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+    <row r="15" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T15" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
-        <v>80631000</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G15" s="7">
-        <v>5.713E-2</v>
-      </c>
-      <c r="H15" s="7">
-        <v>6.6350000000000006E-2</v>
-      </c>
-      <c r="I15" s="7">
-        <v>6.54E-2</v>
-      </c>
-      <c r="J15" s="7">
-        <v>4.7969999999999999E-2</v>
-      </c>
-      <c r="K15" s="7">
-        <v>4.8160000000000001E-2</v>
-      </c>
-      <c r="L15" s="7">
-        <v>4.5749999999999999E-2</v>
-      </c>
-      <c r="M15" s="7">
-        <v>7.306E-2</v>
-      </c>
-      <c r="N15" s="7">
-        <v>7.0499999999999993E-2</v>
-      </c>
-      <c r="O15" s="7">
-        <v>6.5699999999999995E-2</v>
-      </c>
-      <c r="P15" s="7">
-        <v>6.1429999999999998E-2</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>0.14660000000000001</v>
-      </c>
-      <c r="R15" s="7">
-        <v>9.0639999999999998E-2</v>
-      </c>
-      <c r="S15" s="7">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="T15" s="7">
-        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="3:42" x14ac:dyDescent="0.25">
@@ -9053,108 +8974,108 @@
         <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1">
         <v>2020</v>
       </c>
       <c r="G16" s="7">
-        <v>6.1899999999999997E-2</v>
+        <v>5.713E-2</v>
       </c>
       <c r="H16" s="7">
-        <v>7.1800000000000003E-2</v>
+        <v>6.6350000000000006E-2</v>
       </c>
       <c r="I16" s="7">
-        <v>6.9099999999999995E-2</v>
+        <v>6.54E-2</v>
       </c>
       <c r="J16" s="7">
-        <v>5.1240000000000001E-2</v>
+        <v>4.7969999999999999E-2</v>
       </c>
       <c r="K16" s="7">
-        <v>4.446E-2</v>
+        <v>4.8160000000000001E-2</v>
       </c>
       <c r="L16" s="7">
-        <v>8.0439999999999998E-2</v>
+        <v>4.5749999999999999E-2</v>
       </c>
       <c r="M16" s="7">
-        <v>9.3899999999999997E-2</v>
+        <v>7.306E-2</v>
       </c>
       <c r="N16" s="7">
-        <v>7.5130000000000002E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="O16" s="7">
-        <v>6.3600000000000004E-2</v>
+        <v>6.5699999999999995E-2</v>
       </c>
       <c r="P16" s="7">
-        <v>6.1039999999999997E-2</v>
+        <v>6.1429999999999998E-2</v>
       </c>
       <c r="Q16" s="7">
-        <v>0.1278</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="R16" s="7">
-        <v>7.6969999999999997E-2</v>
+        <v>9.0639999999999998E-2</v>
       </c>
       <c r="S16" s="7">
-        <v>7.2900000000000006E-2</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="T16" s="7">
-        <v>4.9840000000000002E-2</v>
+        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
-        <v>80601000</v>
+        <v>80631000</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1">
         <v>2020</v>
       </c>
       <c r="G17" s="7">
-        <v>7.2270000000000001E-2</v>
+        <v>6.1899999999999997E-2</v>
       </c>
       <c r="H17" s="7">
-        <v>8.7160000000000001E-2</v>
+        <v>7.1800000000000003E-2</v>
       </c>
       <c r="I17" s="7">
-        <v>8.0140000000000003E-2</v>
+        <v>6.9099999999999995E-2</v>
       </c>
       <c r="J17" s="7">
-        <v>5.5300000000000002E-2</v>
+        <v>5.1240000000000001E-2</v>
       </c>
       <c r="K17" s="7">
-        <v>5.79E-2</v>
+        <v>4.446E-2</v>
       </c>
       <c r="L17" s="7">
-        <v>4.1930000000000002E-2</v>
+        <v>8.0439999999999998E-2</v>
       </c>
       <c r="M17" s="7">
-        <v>6.9599999999999995E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="N17" s="7">
-        <v>6.2469999999999998E-2</v>
+        <v>7.5130000000000002E-2</v>
       </c>
       <c r="O17" s="7">
-        <v>6.2560000000000004E-2</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="P17" s="7">
-        <v>5.91E-2</v>
+        <v>6.1039999999999997E-2</v>
       </c>
       <c r="Q17" s="7">
-        <v>0.14610000000000001</v>
+        <v>0.1278</v>
       </c>
       <c r="R17" s="7">
-        <v>8.5139999999999993E-2</v>
+        <v>7.6969999999999997E-2</v>
       </c>
       <c r="S17" s="7">
-        <v>7.1900000000000006E-2</v>
+        <v>7.2900000000000006E-2</v>
       </c>
       <c r="T17" s="7">
-        <v>4.8500000000000001E-2</v>
+        <v>4.9840000000000002E-2</v>
       </c>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
@@ -9165,108 +9086,108 @@
         <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1">
         <v>2020</v>
       </c>
       <c r="G18" s="7">
-        <v>7.2139999999999996E-2</v>
+        <v>7.2270000000000001E-2</v>
       </c>
       <c r="H18" s="7">
-        <v>8.6360000000000006E-2</v>
+        <v>8.7160000000000001E-2</v>
       </c>
       <c r="I18" s="7">
-        <v>8.2460000000000006E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="J18" s="7">
-        <v>5.8470000000000001E-2</v>
+        <v>5.5300000000000002E-2</v>
       </c>
       <c r="K18" s="7">
-        <v>6.5250000000000002E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="L18" s="7">
-        <v>5.7099999999999998E-2</v>
+        <v>4.1930000000000002E-2</v>
       </c>
       <c r="M18" s="7">
-        <v>8.0140000000000003E-2</v>
+        <v>6.9599999999999995E-2</v>
       </c>
       <c r="N18" s="7">
-        <v>7.0860000000000006E-2</v>
+        <v>6.2469999999999998E-2</v>
       </c>
       <c r="O18" s="7">
-        <v>5.8900000000000001E-2</v>
+        <v>6.2560000000000004E-2</v>
       </c>
       <c r="P18" s="7">
-        <v>5.8779999999999999E-2</v>
+        <v>5.91E-2</v>
       </c>
       <c r="Q18" s="7">
-        <v>0.1333</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="R18" s="7">
-        <v>7.9000000000000001E-2</v>
+        <v>8.5139999999999993E-2</v>
       </c>
       <c r="S18" s="7">
-        <v>6.1650000000000003E-2</v>
+        <v>7.1900000000000006E-2</v>
       </c>
       <c r="T18" s="7">
-        <v>3.5639999999999998E-2</v>
+        <v>4.8500000000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
-        <v>38701000</v>
+        <v>80601000</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="G19" s="7">
-        <v>4.2900000000000001E-2</v>
+        <v>7.2139999999999996E-2</v>
       </c>
       <c r="H19" s="7">
-        <v>5.9499999999999997E-2</v>
+        <v>8.6360000000000006E-2</v>
       </c>
       <c r="I19" s="7">
-        <v>5.475E-2</v>
+        <v>8.2460000000000006E-2</v>
       </c>
       <c r="J19" s="7">
-        <v>4.8550000000000003E-2</v>
+        <v>5.8470000000000001E-2</v>
       </c>
       <c r="K19" s="7">
-        <v>4.48E-2</v>
+        <v>6.5250000000000002E-2</v>
       </c>
       <c r="L19" s="7">
-        <v>4.9930000000000002E-2</v>
+        <v>5.7099999999999998E-2</v>
       </c>
       <c r="M19" s="7">
-        <v>7.6899999999999996E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="N19" s="7">
-        <v>9.2039999999999997E-2</v>
+        <v>7.0860000000000006E-2</v>
       </c>
       <c r="O19" s="7">
-        <v>8.1799999999999998E-2</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="P19" s="7">
-        <v>7.6100000000000001E-2</v>
+        <v>5.8779999999999999E-2</v>
       </c>
       <c r="Q19" s="7">
-        <v>0.12427000000000001</v>
+        <v>0.1333</v>
       </c>
       <c r="R19" s="7">
-        <v>7.0400000000000004E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="S19" s="7">
-        <v>9.0700000000000003E-2</v>
+        <v>6.1650000000000003E-2</v>
       </c>
       <c r="T19" s="7">
-        <v>8.7340000000000001E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
@@ -9277,108 +9198,108 @@
         <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="1">
         <v>2023</v>
       </c>
       <c r="G20" s="7">
-        <v>5.4960000000000002E-2</v>
+        <v>4.2900000000000001E-2</v>
       </c>
       <c r="H20" s="7">
-        <v>7.3400000000000007E-2</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="I20" s="7">
-        <v>6.744E-2</v>
+        <v>5.475E-2</v>
       </c>
       <c r="J20" s="7">
-        <v>6.1460000000000001E-2</v>
+        <v>4.8550000000000003E-2</v>
       </c>
       <c r="K20" s="7">
-        <v>4.82E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="L20" s="7">
-        <v>5.2060000000000002E-2</v>
+        <v>4.9930000000000002E-2</v>
       </c>
       <c r="M20" s="7">
-        <v>7.9200000000000007E-2</v>
+        <v>7.6899999999999996E-2</v>
       </c>
       <c r="N20" s="7">
-        <v>9.7000000000000003E-2</v>
+        <v>9.2039999999999997E-2</v>
       </c>
       <c r="O20" s="7">
-        <v>8.4839999999999999E-2</v>
+        <v>8.1799999999999998E-2</v>
       </c>
       <c r="P20" s="7">
         <v>7.6100000000000001E-2</v>
       </c>
       <c r="Q20" s="7">
-        <v>0.11269999999999999</v>
+        <v>0.12427000000000001</v>
       </c>
       <c r="R20" s="7">
-        <v>6.1600000000000002E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="S20" s="7">
-        <v>7.1529999999999996E-2</v>
+        <v>9.0700000000000003E-2</v>
       </c>
       <c r="T20" s="7">
-        <v>5.9630000000000002E-2</v>
+        <v>8.7340000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>20627000</v>
+        <v>38701000</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F21" s="1">
-        <v>2012</v>
+        <v>2023</v>
       </c>
       <c r="G21" s="7">
-        <v>5.9569999999999998E-2</v>
+        <v>5.4960000000000002E-2</v>
       </c>
       <c r="H21" s="7">
-        <v>5.3039999999999997E-2</v>
+        <v>7.3400000000000007E-2</v>
       </c>
       <c r="I21" s="7">
-        <v>5.57E-2</v>
+        <v>6.744E-2</v>
       </c>
       <c r="J21" s="7">
-        <v>5.1450000000000003E-2</v>
+        <v>6.1460000000000001E-2</v>
       </c>
       <c r="K21" s="7">
-        <v>6.5369999999999998E-2</v>
+        <v>4.82E-2</v>
       </c>
       <c r="L21" s="7">
-        <v>7.7899999999999997E-2</v>
+        <v>5.2060000000000002E-2</v>
       </c>
       <c r="M21" s="7">
-        <v>7.6899999999999996E-2</v>
+        <v>7.9200000000000007E-2</v>
       </c>
       <c r="N21" s="7">
-        <v>7.6999999999999999E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="O21" s="7">
-        <v>7.4999999999999997E-2</v>
+        <v>8.4839999999999999E-2</v>
       </c>
       <c r="P21" s="7">
-        <v>8.6099999999999996E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="Q21" s="7">
-        <v>0.10284</v>
+        <v>0.11269999999999999</v>
       </c>
       <c r="R21" s="7">
-        <v>8.9099999999999999E-2</v>
+        <v>6.1600000000000002E-2</v>
       </c>
       <c r="S21" s="7">
-        <v>8.5599999999999996E-2</v>
+        <v>7.1529999999999996E-2</v>
       </c>
       <c r="T21" s="7">
-        <v>4.4400000000000002E-2</v>
+        <v>5.9630000000000002E-2</v>
       </c>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
@@ -9389,108 +9310,108 @@
         <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="1">
         <v>2012</v>
       </c>
       <c r="G22" s="7">
-        <v>6.1280000000000001E-2</v>
+        <v>5.9569999999999998E-2</v>
       </c>
       <c r="H22" s="7">
-        <v>5.9360000000000003E-2</v>
+        <v>5.3039999999999997E-2</v>
       </c>
       <c r="I22" s="7">
-        <v>6.4899999999999999E-2</v>
+        <v>5.57E-2</v>
       </c>
       <c r="J22" s="7">
-        <v>6.3600000000000004E-2</v>
+        <v>5.1450000000000003E-2</v>
       </c>
       <c r="K22" s="7">
-        <v>7.1400000000000005E-2</v>
+        <v>6.5369999999999998E-2</v>
       </c>
       <c r="L22" s="7">
-        <v>8.8599999999999998E-2</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="M22" s="7">
-        <v>7.6700000000000004E-2</v>
+        <v>7.6899999999999996E-2</v>
       </c>
       <c r="N22" s="7">
-        <v>7.6300000000000007E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O22" s="7">
-        <v>7.4300000000000005E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="P22" s="7">
-        <v>8.6300000000000002E-2</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="Q22" s="7">
-        <v>0.10297000000000001</v>
+        <v>0.10284</v>
       </c>
       <c r="R22" s="7">
-        <v>8.0699999999999994E-2</v>
+        <v>8.9099999999999999E-2</v>
       </c>
       <c r="S22" s="7">
-        <v>6.6650000000000001E-2</v>
+        <v>8.5599999999999996E-2</v>
       </c>
       <c r="T22" s="7">
-        <v>2.6980000000000001E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>92634000</v>
+        <v>20627000</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1">
-        <v>2020</v>
+        <v>2012</v>
       </c>
       <c r="G23" s="7">
-        <v>6.1769999999999999E-2</v>
+        <v>6.1280000000000001E-2</v>
       </c>
       <c r="H23" s="7">
-        <v>6.7199999999999996E-2</v>
+        <v>5.9360000000000003E-2</v>
       </c>
       <c r="I23" s="7">
-        <v>5.21E-2</v>
+        <v>6.4899999999999999E-2</v>
       </c>
       <c r="J23" s="7">
-        <v>4.675E-2</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="K23" s="7">
-        <v>4.8070000000000002E-2</v>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="L23" s="7">
-        <v>7.0599999999999996E-2</v>
+        <v>8.8599999999999998E-2</v>
       </c>
       <c r="M23" s="7">
-        <v>9.35E-2</v>
+        <v>7.6700000000000004E-2</v>
       </c>
       <c r="N23" s="7">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="O23" s="7">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="P23" s="7">
+        <v>8.6300000000000002E-2</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0.10297000000000001</v>
+      </c>
+      <c r="R23" s="7">
         <v>8.0699999999999994E-2</v>
       </c>
-      <c r="O23" s="7">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="P23" s="7">
-        <v>5.9080000000000001E-2</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>0.12870000000000001</v>
-      </c>
-      <c r="R23" s="7">
-        <v>7.7759999999999996E-2</v>
-      </c>
       <c r="S23" s="7">
-        <v>8.4659999999999999E-2</v>
+        <v>6.6650000000000001E-2</v>
       </c>
       <c r="T23" s="7">
-        <v>6.1519999999999998E-2</v>
+        <v>2.6980000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
@@ -9501,108 +9422,108 @@
         <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="1">
         <v>2020</v>
       </c>
       <c r="G24" s="7">
-        <v>6.7500000000000004E-2</v>
+        <v>6.1769999999999999E-2</v>
       </c>
       <c r="H24" s="7">
-        <v>7.6050000000000006E-2</v>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="I24" s="7">
-        <v>5.7860000000000002E-2</v>
+        <v>5.21E-2</v>
       </c>
       <c r="J24" s="7">
-        <v>4.8829999999999998E-2</v>
+        <v>4.675E-2</v>
       </c>
       <c r="K24" s="7">
-        <v>4.376E-2</v>
+        <v>4.8070000000000002E-2</v>
       </c>
       <c r="L24" s="7">
-        <v>7.7299999999999994E-2</v>
+        <v>7.0599999999999996E-2</v>
       </c>
       <c r="M24" s="7">
-        <v>0.10564999999999999</v>
+        <v>9.35E-2</v>
       </c>
       <c r="N24" s="7">
-        <v>8.0750000000000002E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="O24" s="7">
-        <v>7.22E-2</v>
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="P24" s="7">
-        <v>5.8779999999999999E-2</v>
+        <v>5.9080000000000001E-2</v>
       </c>
       <c r="Q24" s="7">
-        <v>0.11940000000000001</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="R24" s="7">
-        <v>7.0739999999999997E-2</v>
+        <v>7.7759999999999996E-2</v>
       </c>
       <c r="S24" s="7">
-        <v>7.2139999999999996E-2</v>
+        <v>8.4659999999999999E-2</v>
       </c>
       <c r="T24" s="7">
-        <v>4.9160000000000002E-2</v>
+        <v>6.1519999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>3703000</v>
+        <v>92634000</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F25" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="G25" s="7">
-        <v>6.0760000000000002E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="H25" s="7">
-        <v>6.207E-2</v>
+        <v>7.6050000000000006E-2</v>
       </c>
       <c r="I25" s="7">
-        <v>5.2670000000000002E-2</v>
+        <v>5.7860000000000002E-2</v>
       </c>
       <c r="J25" s="7">
-        <v>4.6539999999999998E-2</v>
+        <v>4.8829999999999998E-2</v>
       </c>
       <c r="K25" s="7">
-        <v>3.8420000000000003E-2</v>
+        <v>4.376E-2</v>
       </c>
       <c r="L25" s="7">
-        <v>5.6599999999999998E-2</v>
+        <v>7.7299999999999994E-2</v>
       </c>
       <c r="M25" s="7">
-        <v>8.0299999999999996E-2</v>
+        <v>0.10564999999999999</v>
       </c>
       <c r="N25" s="7">
-        <v>8.8440000000000005E-2</v>
+        <v>8.0750000000000002E-2</v>
       </c>
       <c r="O25" s="7">
-        <v>7.8899999999999998E-2</v>
+        <v>7.22E-2</v>
       </c>
       <c r="P25" s="7">
-        <v>7.0499999999999993E-2</v>
+        <v>5.8779999999999999E-2</v>
       </c>
       <c r="Q25" s="7">
-        <v>0.1244</v>
+        <v>0.11940000000000001</v>
       </c>
       <c r="R25" s="7">
-        <v>7.6050000000000006E-2</v>
+        <v>7.0739999999999997E-2</v>
       </c>
       <c r="S25" s="7">
-        <v>8.7599999999999997E-2</v>
+        <v>7.2139999999999996E-2</v>
       </c>
       <c r="T25" s="7">
-        <v>7.6799999999999993E-2</v>
+        <v>4.9160000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
@@ -9610,111 +9531,111 @@
         <v>3703000</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="1">
         <v>2021</v>
       </c>
       <c r="G26" s="7">
-        <v>7.1840000000000001E-2</v>
+        <v>6.0760000000000002E-2</v>
       </c>
       <c r="H26" s="7">
-        <v>7.4300000000000005E-2</v>
+        <v>6.207E-2</v>
       </c>
       <c r="I26" s="7">
-        <v>6.4699999999999994E-2</v>
+        <v>5.2670000000000002E-2</v>
       </c>
       <c r="J26" s="7">
-        <v>5.2600000000000001E-2</v>
+        <v>4.6539999999999998E-2</v>
       </c>
       <c r="K26" s="7">
-        <v>4.1320000000000003E-2</v>
+        <v>3.8420000000000003E-2</v>
       </c>
       <c r="L26" s="7">
-        <v>6.93E-2</v>
+        <v>5.6599999999999998E-2</v>
       </c>
       <c r="M26" s="7">
-        <v>8.9539999999999995E-2</v>
+        <v>8.0299999999999996E-2</v>
       </c>
       <c r="N26" s="7">
-        <v>8.4099999999999994E-2</v>
+        <v>8.8440000000000005E-2</v>
       </c>
       <c r="O26" s="7">
-        <v>7.6539999999999997E-2</v>
+        <v>7.8899999999999998E-2</v>
       </c>
       <c r="P26" s="7">
-        <v>6.9800000000000001E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="Q26" s="7">
-        <v>0.11053</v>
+        <v>0.1244</v>
       </c>
       <c r="R26" s="7">
-        <v>6.5100000000000005E-2</v>
+        <v>7.6050000000000006E-2</v>
       </c>
       <c r="S26" s="7">
-        <v>7.0400000000000004E-2</v>
+        <v>8.7599999999999997E-2</v>
       </c>
       <c r="T26" s="7">
-        <v>5.9970000000000002E-2</v>
+        <v>7.6799999999999993E-2</v>
       </c>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>3708000</v>
+        <v>3703000</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F27" s="1">
         <v>2021</v>
       </c>
       <c r="G27" s="7">
-        <v>5.774E-2</v>
+        <v>7.1840000000000001E-2</v>
       </c>
       <c r="H27" s="7">
-        <v>6.0199999999999997E-2</v>
+        <v>7.4300000000000005E-2</v>
       </c>
       <c r="I27" s="7">
-        <v>5.1479999999999998E-2</v>
+        <v>6.4699999999999994E-2</v>
       </c>
       <c r="J27" s="7">
-        <v>4.2569999999999997E-2</v>
+        <v>5.2600000000000001E-2</v>
       </c>
       <c r="K27" s="7">
-        <v>3.5430000000000003E-2</v>
+        <v>4.1320000000000003E-2</v>
       </c>
       <c r="L27" s="7">
-        <v>4.437E-2</v>
+        <v>6.93E-2</v>
       </c>
       <c r="M27" s="7">
-        <v>8.0140000000000003E-2</v>
+        <v>8.9539999999999995E-2</v>
       </c>
       <c r="N27" s="7">
-        <v>9.2499999999999999E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
       <c r="O27" s="7">
-        <v>8.3599999999999994E-2</v>
+        <v>7.6539999999999997E-2</v>
       </c>
       <c r="P27" s="7">
-        <v>7.4700000000000003E-2</v>
+        <v>6.9800000000000001E-2</v>
       </c>
       <c r="Q27" s="7">
-        <v>0.13100000000000001</v>
+        <v>0.11053</v>
       </c>
       <c r="R27" s="7">
-        <v>7.8299999999999995E-2</v>
+        <v>6.5100000000000005E-2</v>
       </c>
       <c r="S27" s="7">
-        <v>8.8900000000000007E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="T27" s="7">
-        <v>7.9039999999999999E-2</v>
+        <v>5.9970000000000002E-2</v>
       </c>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
@@ -9722,122 +9643,223 @@
         <v>3708000</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F28" s="1">
         <v>2021</v>
       </c>
       <c r="G28" s="7">
+        <v>5.774E-2</v>
+      </c>
+      <c r="H28" s="7">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="I28" s="7">
+        <v>5.1479999999999998E-2</v>
+      </c>
+      <c r="J28" s="7">
+        <v>4.2569999999999997E-2</v>
+      </c>
+      <c r="K28" s="7">
+        <v>3.5430000000000003E-2</v>
+      </c>
+      <c r="L28" s="7">
+        <v>4.437E-2</v>
+      </c>
+      <c r="M28" s="7">
+        <v>8.0140000000000003E-2</v>
+      </c>
+      <c r="N28" s="7">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="O28" s="7">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="P28" s="7">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="R28" s="7">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="S28" s="7">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="T28" s="7">
+        <v>7.9039999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>3708000</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G29" s="7">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H29" s="7">
         <v>7.2749999999999995E-2</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I29" s="7">
         <v>6.1830000000000003E-2</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J29" s="7">
         <v>5.0659999999999997E-2</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K29" s="7">
         <v>4.0399999999999998E-2</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L29" s="7">
         <v>5.3220000000000003E-2</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M29" s="7">
         <v>8.0750000000000002E-2</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N29" s="7">
         <v>9.1740000000000002E-2</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O29" s="7">
         <v>8.5629999999999998E-2</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P29" s="7">
         <v>7.1349999999999997E-2</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q29" s="7">
         <v>0.11890000000000001</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R29" s="7">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="S28" s="7">
+      <c r="S29" s="7">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T29" s="7">
         <v>6.2799999999999995E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="1" t="s">
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>25703000</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="7">
-        <f>AVERAGE(G15,G17,G19,G21)</f>
-        <v>5.7967500000000005E-2</v>
-      </c>
-      <c r="H33" s="7">
-        <f>AVERAGE(H15,H17,H19,H21)</f>
-        <v>6.6512500000000002E-2</v>
-      </c>
-      <c r="I33" s="7">
-        <f>AVERAGE(I15,I17,I19,I21)</f>
-        <v>6.3997499999999999E-2</v>
-      </c>
-      <c r="J33" s="7">
-        <f>AVERAGE(J15,J17,J19,J21)</f>
-        <v>5.0817500000000002E-2</v>
-      </c>
-      <c r="K33" s="7">
-        <f>AVERAGE(K15,K17,K19,K21)</f>
-        <v>5.4057499999999994E-2</v>
-      </c>
-      <c r="L33" s="7">
-        <f>AVERAGE(L15,L17,L19,L21)</f>
-        <v>5.3877500000000002E-2</v>
-      </c>
-      <c r="M33" s="7">
-        <f>AVERAGE(M15,M17,M19,M21)</f>
-        <v>7.4115E-2</v>
-      </c>
-      <c r="N33" s="7">
-        <f>AVERAGE(N15,N17,N19,N21)</f>
-        <v>7.55025E-2</v>
-      </c>
-      <c r="O33" s="7">
-        <f>AVERAGE(O15,O17,O19,O21)</f>
-        <v>7.1264999999999995E-2</v>
-      </c>
-      <c r="P33" s="7">
-        <f>AVERAGE(P15,P17,P19,P21)</f>
-        <v>7.0682499999999995E-2</v>
-      </c>
-      <c r="Q33" s="7">
-        <f>AVERAGE(Q15,Q17,Q19,Q21)</f>
-        <v>0.1299525</v>
-      </c>
-      <c r="R33" s="7">
-        <f>AVERAGE(R15,R17,R19,R21)</f>
-        <v>8.3820000000000006E-2</v>
-      </c>
-      <c r="S33" s="7">
-        <f>AVERAGE(S15,S17,S19,S21)</f>
-        <v>8.3925E-2</v>
-      </c>
-      <c r="T33" s="7">
-        <f>AVERAGE(T15,T17,T19,T21)</f>
-        <v>6.3485E-2</v>
+      <c r="F30" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G30" s="7">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="H30" s="7">
+        <v>6.5729999999999997E-2</v>
+      </c>
+      <c r="I30" s="7">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="J30" s="7">
+        <v>4.904E-2</v>
+      </c>
+      <c r="K30" s="7">
+        <v>4.4220000000000002E-2</v>
+      </c>
+      <c r="L30" s="7">
+        <v>6.0639999999999999E-2</v>
+      </c>
+      <c r="M30" s="7">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="N30" s="7">
+        <v>8.48E-2</v>
+      </c>
+      <c r="O30" s="7">
+        <v>7.6350000000000001E-2</v>
+      </c>
+      <c r="P30" s="7">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>0.12256</v>
+      </c>
+      <c r="R30" s="7">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="S30" s="7">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="T30" s="7">
+        <v>7.1529999999999996E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>25703000</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G31" s="7">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="H31" s="7">
+        <v>7.3499999999999996E-2</v>
+      </c>
+      <c r="I31" s="7">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="J31" s="7">
+        <v>5.7619999999999998E-2</v>
+      </c>
+      <c r="K31" s="7">
+        <v>5.28E-2</v>
+      </c>
+      <c r="L31" s="7">
+        <v>7.2139999999999996E-2</v>
+      </c>
+      <c r="M31" s="7">
+        <v>0.10266</v>
+      </c>
+      <c r="N31" s="7">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="O31" s="7">
+        <v>7.8060000000000004E-2</v>
+      </c>
+      <c r="P31" s="7">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="R31" s="7">
+        <v>6.0850000000000001E-2</v>
+      </c>
+      <c r="S31" s="7">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="T31" s="7">
+        <v>4.3099999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="3:22" x14ac:dyDescent="0.25">
@@ -9845,187 +9867,195 @@
         <v>43</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
       </c>
       <c r="G34" s="7">
-        <f>AVERAGE(G16,G18,G20,G22)</f>
-        <v>6.2570000000000001E-2</v>
+        <f>AVERAGE(G16,G18,G20,G22,G24,G26,G28,G30)</f>
+        <v>5.883E-2</v>
       </c>
       <c r="H34" s="7">
-        <f>AVERAGE(H16,H18,H20,H22)</f>
-        <v>7.2730000000000017E-2</v>
+        <f t="shared" ref="H34:T34" si="1">AVERAGE(H16,H18,H20,H22,H24,H26,H28,H30)</f>
+        <v>6.5156249999999999E-2</v>
       </c>
       <c r="I34" s="7">
-        <f>AVERAGE(I16,I18,I20,I22)</f>
-        <v>7.0974999999999996E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.8517499999999993E-2</v>
       </c>
       <c r="J34" s="7">
-        <f>AVERAGE(J16,J18,J20,J22)</f>
-        <v>5.8692499999999995E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.8521250000000002E-2</v>
       </c>
       <c r="K34" s="7">
-        <f>AVERAGE(K16,K18,K20,K22)</f>
-        <v>5.7327500000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7796249999999998E-2</v>
       </c>
       <c r="L34" s="7">
-        <f>AVERAGE(L16,L18,L20,L22)</f>
-        <v>6.9550000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.5965000000000001E-2</v>
       </c>
       <c r="M34" s="7">
-        <f>AVERAGE(M16,M18,M20,M22)</f>
-        <v>8.2485000000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.9662499999999997E-2</v>
       </c>
       <c r="N34" s="7">
-        <f>AVERAGE(N16,N18,N20,N22)</f>
-        <v>7.9822500000000005E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.1056249999999996E-2</v>
       </c>
       <c r="O34" s="7">
-        <f>AVERAGE(O16,O18,O20,O22)</f>
-        <v>7.041E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.3938749999999998E-2</v>
       </c>
       <c r="P34" s="7">
-        <f>AVERAGE(P16,P18,P20,P22)</f>
-        <v>7.0554999999999993E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.9988750000000002E-2</v>
       </c>
       <c r="Q34" s="7">
-        <f>AVERAGE(Q16,Q18,Q20,Q22)</f>
-        <v>0.11919250000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.12830875</v>
       </c>
       <c r="R34" s="7">
-        <f>AVERAGE(R16,R18,R20,R22)</f>
-        <v>7.4567499999999995E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.0073750000000013E-2</v>
       </c>
       <c r="S34" s="7">
-        <f>AVERAGE(S16,S18,S20,S22)</f>
-        <v>6.8182499999999993E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.4332499999999991E-2</v>
       </c>
       <c r="T34" s="7">
-        <f>AVERAGE(T16,T18,T20,T22)</f>
-        <v>4.3022500000000005E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.7853750000000004E-2</v>
       </c>
     </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="2" t="s">
+    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="1">
         <v>0</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V39" s="2" t="s">
-        <v>16</v>
+      <c r="G35" s="7">
+        <f>AVERAGE(G17,G19,G21,G23,G25,G27,G29,G31)</f>
+        <v>6.5652500000000003E-2</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" ref="H35:T35" si="2">AVERAGE(H17,H19,H21,H23,H25,H27,H29,H31)</f>
+        <v>7.3440000000000005E-2</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="2"/>
+        <v>6.6498749999999995E-2</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="2"/>
+        <v>5.5559999999999991E-2</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="2"/>
+        <v>5.0948750000000008E-2</v>
+      </c>
+      <c r="L35" s="7">
+        <f t="shared" si="2"/>
+        <v>6.8769999999999998E-2</v>
+      </c>
+      <c r="M35" s="7">
+        <f t="shared" si="2"/>
+        <v>8.8567499999999993E-2</v>
+      </c>
+      <c r="N35" s="7">
+        <f t="shared" si="2"/>
+        <v>8.40225E-2</v>
+      </c>
+      <c r="O35" s="7">
+        <f t="shared" si="2"/>
+        <v>7.4258749999999998E-2</v>
+      </c>
+      <c r="P35" s="7">
+        <f t="shared" si="2"/>
+        <v>6.9218749999999996E-2</v>
+      </c>
+      <c r="Q35" s="7">
+        <f t="shared" si="2"/>
+        <v>0.11650000000000002</v>
+      </c>
+      <c r="R35" s="7">
+        <f t="shared" si="2"/>
+        <v>7.048249999999999E-2</v>
+      </c>
+      <c r="S35" s="7">
+        <f t="shared" si="2"/>
+        <v>6.7721249999999997E-2</v>
+      </c>
+      <c r="T35" s="7">
+        <f t="shared" si="2"/>
+        <v>4.8390000000000002E-2</v>
       </c>
     </row>
     <row r="40" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="1">
-        <v>2015</v>
-      </c>
-      <c r="F40" s="1">
-        <v>-508</v>
-      </c>
-      <c r="G40" s="1">
-        <v>89673</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0.17097677115742749</v>
-      </c>
-      <c r="I40" s="1">
-        <v>20274.726180000001</v>
-      </c>
-      <c r="J40" s="1">
-        <v>0.63144982324668508</v>
-      </c>
-      <c r="K40" s="1">
-        <v>1.8846252495176911E-2</v>
-      </c>
-      <c r="L40" s="1">
-        <v>23.73828289719313</v>
-      </c>
-      <c r="M40" s="1">
-        <v>25.6</v>
-      </c>
-      <c r="N40" s="1">
-        <v>5.8769083224604586E-3</v>
-      </c>
-      <c r="O40" s="1">
-        <v>2.9663332329686628E-3</v>
-      </c>
-      <c r="P40" s="1">
-        <v>8.227671651444687E-3</v>
-      </c>
-      <c r="Q40" s="1">
-        <v>1.0814961025057701</v>
-      </c>
-      <c r="R40" s="1">
-        <v>0.67026351298607134</v>
-      </c>
-      <c r="S40" s="1">
-        <v>25.881326426014489</v>
-      </c>
-      <c r="T40" s="1">
-        <v>4.9067166259632105E-4</v>
-      </c>
-      <c r="U40" s="1">
-        <v>5.6929064489868737E-2</v>
-      </c>
-      <c r="V40" s="1">
-        <v>119.345016326319</v>
+      <c r="C40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.25">
@@ -10033,58 +10063,58 @@
         <v>51</v>
       </c>
       <c r="E41" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="F41" s="1">
-        <v>-583</v>
+        <v>-508</v>
       </c>
       <c r="G41" s="1">
-        <v>88968</v>
+        <v>89673</v>
       </c>
       <c r="H41" s="1">
-        <v>0.1689259059437101</v>
+        <v>0.17097677115742749</v>
       </c>
       <c r="I41" s="1">
-        <v>21016.71081</v>
+        <v>20274.726180000001</v>
       </c>
       <c r="J41" s="1">
-        <v>0.63645580433414262</v>
+        <v>0.63144982324668508</v>
       </c>
       <c r="K41" s="1">
-        <v>1.899559392140994E-2</v>
+        <v>1.8846252495176911E-2</v>
       </c>
       <c r="L41" s="1">
-        <v>23.527577473473599</v>
+        <v>23.73828289719313</v>
       </c>
       <c r="M41" s="1">
-        <v>26.6</v>
+        <v>25.6</v>
       </c>
       <c r="N41" s="1">
-        <v>5.9234781044869714E-3</v>
+        <v>5.8769083224604586E-3</v>
       </c>
       <c r="O41" s="1">
-        <v>3.0572790216706999E-3</v>
+        <v>2.9663332329686628E-3</v>
       </c>
       <c r="P41" s="1">
-        <v>8.4412372988040517E-3</v>
+        <v>8.227671651444687E-3</v>
       </c>
       <c r="Q41" s="1">
-        <v>1.082479093606689</v>
+        <v>1.0814961025057701</v>
       </c>
       <c r="R41" s="1">
-        <v>0.61311033180469354</v>
+        <v>0.67026351298607134</v>
       </c>
       <c r="S41" s="1">
-        <v>24.770910734196551</v>
+        <v>25.881326426014489</v>
       </c>
       <c r="T41" s="1">
-        <v>4.9455984174084965E-4</v>
+        <v>4.9067166259632105E-4</v>
       </c>
       <c r="U41" s="1">
-        <v>5.7874741480082717E-2</v>
+        <v>5.6929064489868737E-2</v>
       </c>
       <c r="V41" s="1">
-        <v>143.61354485994971</v>
+        <v>119.345016326319</v>
       </c>
     </row>
     <row r="42" spans="3:22" x14ac:dyDescent="0.25">
@@ -10092,58 +10122,58 @@
         <v>51</v>
       </c>
       <c r="E42" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F42" s="1">
-        <v>-507</v>
+        <v>-583</v>
       </c>
       <c r="G42" s="1">
-        <v>88092</v>
+        <v>88968</v>
       </c>
       <c r="H42" s="1">
-        <v>0.1657471734096172</v>
+        <v>0.1689259059437101</v>
       </c>
       <c r="I42" s="1">
-        <v>22275.830239999999</v>
+        <v>21016.71081</v>
       </c>
       <c r="J42" s="1">
-        <v>0.67765063796939562</v>
+        <v>0.63645580433414262</v>
       </c>
       <c r="K42" s="1">
-        <v>1.9740725605049251E-2</v>
+        <v>1.899559392140994E-2</v>
       </c>
       <c r="L42" s="1">
-        <v>26.707001895631841</v>
+        <v>23.527577473473599</v>
       </c>
       <c r="M42" s="1">
-        <v>27.4</v>
+        <v>26.6</v>
       </c>
       <c r="N42" s="1">
-        <v>5.9823820551241514E-3</v>
+        <v>5.9234781044869714E-3</v>
       </c>
       <c r="O42" s="1">
-        <v>3.0536257548926002E-3</v>
+        <v>3.0572790216706999E-3</v>
       </c>
       <c r="P42" s="1">
-        <v>8.7851337238341615E-3</v>
+        <v>8.4412372988040517E-3</v>
       </c>
       <c r="Q42" s="1">
-        <v>1.0234073468646401</v>
+        <v>1.082479093606689</v>
       </c>
       <c r="R42" s="1">
-        <v>0.61994051673250683</v>
+        <v>0.61311033180469354</v>
       </c>
       <c r="S42" s="1">
-        <v>21.178866225082849</v>
+        <v>24.770910734196551</v>
       </c>
       <c r="T42" s="1">
-        <v>4.9947781864414359E-4</v>
+        <v>4.9455984174084965E-4</v>
       </c>
       <c r="U42" s="1">
-        <v>5.87113472278981E-2</v>
+        <v>5.7874741480082717E-2</v>
       </c>
       <c r="V42" s="1">
-        <v>142.04406721007581</v>
+        <v>143.61354485994971</v>
       </c>
     </row>
     <row r="43" spans="3:22" x14ac:dyDescent="0.25">
@@ -10151,244 +10181,241 @@
         <v>51</v>
       </c>
       <c r="E43" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F43" s="1">
-        <v>-711</v>
+        <v>-507</v>
       </c>
       <c r="G43" s="1">
-        <v>87282</v>
+        <v>88092</v>
       </c>
       <c r="H43" s="1">
-        <v>0.16122453655965721</v>
+        <v>0.1657471734096172</v>
       </c>
       <c r="I43" s="1">
-        <v>23989.908439999999</v>
+        <v>22275.830239999999</v>
       </c>
       <c r="J43" s="1">
-        <v>0.68737654957494088</v>
+        <v>0.67765063796939562</v>
       </c>
       <c r="K43" s="1">
-        <v>1.875529891615681E-2</v>
+        <v>1.9740725605049251E-2</v>
       </c>
       <c r="L43" s="1">
-        <v>29.351305275772781</v>
+        <v>26.707001895631841</v>
       </c>
       <c r="M43" s="1">
-        <v>28.1</v>
+        <v>27.4</v>
       </c>
       <c r="N43" s="1">
-        <v>6.3586993881899652E-3</v>
+        <v>5.9823820551241514E-3</v>
       </c>
       <c r="O43" s="1">
-        <v>3.0819642079695569E-3</v>
+        <v>3.0536257548926002E-3</v>
       </c>
       <c r="P43" s="1">
-        <v>9.3810865928828282E-3</v>
+        <v>8.7851337238341615E-3</v>
       </c>
       <c r="Q43" s="1">
-        <v>0.98409752297151609</v>
+        <v>1.0234073468646401</v>
       </c>
       <c r="R43" s="1">
-        <v>0.71611913109232095</v>
+        <v>0.61994051673250683</v>
       </c>
       <c r="S43" s="1">
-        <v>20.416691414037231</v>
+        <v>21.178866225082849</v>
       </c>
       <c r="T43" s="1">
-        <v>5.0411310464929633E-4</v>
+        <v>4.9947781864414359E-4</v>
       </c>
       <c r="U43" s="1">
-        <v>5.925620402832199E-2</v>
+        <v>5.87113472278981E-2</v>
       </c>
       <c r="V43" s="1">
-        <v>145.038276238858</v>
+        <v>142.04406721007581</v>
       </c>
     </row>
     <row r="44" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-711</v>
+      </c>
+      <c r="G44" s="1">
+        <v>87282</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.16122453655965721</v>
+      </c>
+      <c r="I44" s="1">
+        <v>23989.908439999999</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.68737654957494088</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1.875529891615681E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <v>29.351305275772781</v>
+      </c>
+      <c r="M44" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="N44" s="1">
+        <v>6.3586993881899652E-3</v>
+      </c>
+      <c r="O44" s="1">
+        <v>3.0819642079695569E-3</v>
+      </c>
+      <c r="P44" s="1">
+        <v>9.3810865928828282E-3</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0.98409752297151609</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0.71611913109232095</v>
+      </c>
+      <c r="S44" s="1">
+        <v>20.416691414037231</v>
+      </c>
+      <c r="T44" s="1">
+        <v>5.0411310464929633E-4</v>
+      </c>
+      <c r="U44" s="1">
+        <v>5.925620402832199E-2</v>
+      </c>
+      <c r="V44" s="1">
+        <v>145.038276238858</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E45" s="3">
         <v>2020</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F45" s="1">
         <v>-151.99999999999989</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G45" s="1">
         <v>85939</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H45" s="1">
         <v>0.15749543280699099</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I45" s="1">
         <v>24720.091919999999</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J45" s="1">
         <v>0.81039690943576237</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K45" s="1">
         <v>1.8396769801836171E-2</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L45" s="1">
         <v>32.194688077822633</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M45" s="1">
         <v>28.7</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N45" s="1">
         <v>6.539522219248496E-3</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O45" s="1">
         <v>2.5715914776760149E-3</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P45" s="1">
         <v>1.0555161219004169E-2</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="Q45" s="1">
         <v>1.1495013905211819</v>
       </c>
-      <c r="R44" s="1">
+      <c r="R45" s="1">
         <v>0.66520904362396571</v>
       </c>
-      <c r="S44" s="1">
+      <c r="S45" s="1">
         <v>22.581482595794672</v>
       </c>
-      <c r="T44" s="1">
+      <c r="T45" s="1">
         <v>7.4471427407812321E-4</v>
       </c>
-      <c r="U44" s="1">
+      <c r="U45" s="1">
         <v>6.0112405310743661E-2</v>
       </c>
-      <c r="V44" s="1">
+      <c r="V45" s="1">
         <v>153.74505778284589</v>
-      </c>
-    </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C47" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S47" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V47" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="48" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C48" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="1">
-        <v>2015</v>
-      </c>
-      <c r="F48" s="1">
-        <v>-163</v>
-      </c>
-      <c r="G48" s="1">
-        <v>44795</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0.1195669159504409</v>
-      </c>
-      <c r="I48" s="1">
-        <v>19632.524519999999</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0.26123004799642802</v>
-      </c>
-      <c r="K48" s="1">
-        <v>3.0717714030583751E-2</v>
-      </c>
-      <c r="L48" s="1">
-        <v>6.8428243203482468</v>
-      </c>
-      <c r="M48" s="1">
-        <v>25.4</v>
-      </c>
-      <c r="N48" s="1">
-        <v>3.415559772295994E-3</v>
-      </c>
-      <c r="O48" s="1">
-        <v>2.2993637682777002E-3</v>
-      </c>
-      <c r="P48" s="1">
-        <v>1.320683111954458E-2</v>
-      </c>
-      <c r="Q48" s="1">
-        <v>3.216117870298024</v>
-      </c>
-      <c r="R48" s="1">
-        <v>0.54021386315436981</v>
-      </c>
-      <c r="S48" s="1">
-        <v>65.877446219444096</v>
-      </c>
-      <c r="T48" s="1">
-        <v>1.5626744056256249E-3</v>
-      </c>
-      <c r="U48" s="1">
-        <v>4.6790936488447371E-2</v>
-      </c>
-      <c r="V48" s="1">
-        <v>36.086993072441103</v>
+      <c r="C48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V48" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="3:22" x14ac:dyDescent="0.25">
@@ -10399,58 +10426,58 @@
         <v>52</v>
       </c>
       <c r="E49" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="F49" s="1">
-        <v>-100</v>
+        <v>-163</v>
       </c>
       <c r="G49" s="1">
-        <v>44888</v>
+        <v>44795</v>
       </c>
       <c r="H49" s="1">
-        <v>0.1251559436820531</v>
+        <v>0.1195669159504409</v>
       </c>
       <c r="I49" s="1">
-        <v>18340.544890000001</v>
+        <v>19632.524519999999</v>
       </c>
       <c r="J49" s="1">
-        <v>0.37225984672963802</v>
+        <v>0.26123004799642802</v>
       </c>
       <c r="K49" s="1">
-        <v>3.412938870076633E-2</v>
+        <v>3.0717714030583751E-2</v>
       </c>
       <c r="L49" s="1">
-        <v>8.4181796671716178</v>
+        <v>6.8428243203482468</v>
       </c>
       <c r="M49" s="1">
-        <v>27.3</v>
+        <v>25.4</v>
       </c>
       <c r="N49" s="1">
-        <v>3.2970949919800181E-3</v>
+        <v>3.415559772295994E-3</v>
       </c>
       <c r="O49" s="1">
-        <v>2.31687756193191E-3</v>
+        <v>2.2993637682777002E-3</v>
       </c>
       <c r="P49" s="1">
-        <v>1.3460167528069861E-2</v>
+        <v>1.320683111954458E-2</v>
       </c>
       <c r="Q49" s="1">
-        <v>3.237123507396185</v>
+        <v>3.216117870298024</v>
       </c>
       <c r="R49" s="1">
-        <v>0.44668731063981459</v>
+        <v>0.54021386315436981</v>
       </c>
       <c r="S49" s="1">
-        <v>65.029295230351053</v>
+        <v>65.877446219444096</v>
       </c>
       <c r="T49" s="1">
-        <v>1.559436820531096E-3</v>
+        <v>1.5626744056256249E-3</v>
       </c>
       <c r="U49" s="1">
-        <v>4.7696489039386912E-2</v>
+        <v>4.6790936488447371E-2</v>
       </c>
       <c r="V49" s="1">
-        <v>36.327307061575482</v>
+        <v>36.086993072441103</v>
       </c>
     </row>
     <row r="50" spans="3:22" x14ac:dyDescent="0.25">
@@ -10461,58 +10488,58 @@
         <v>52</v>
       </c>
       <c r="E50" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F50" s="1">
-        <v>-179</v>
+        <v>-100</v>
       </c>
       <c r="G50" s="1">
-        <v>44962</v>
+        <v>44888</v>
       </c>
       <c r="H50" s="1">
-        <v>0.1264401049775366</v>
+        <v>0.1251559436820531</v>
       </c>
       <c r="I50" s="1">
-        <v>19591.68519</v>
+        <v>18340.544890000001</v>
       </c>
       <c r="J50" s="1">
-        <v>0.37287042391352693</v>
+        <v>0.37225984672963802</v>
       </c>
       <c r="K50" s="1">
-        <v>3.0603620835372079E-2</v>
+        <v>3.412938870076633E-2</v>
       </c>
       <c r="L50" s="1">
-        <v>22.083162368444469</v>
+        <v>8.4181796671716178</v>
       </c>
       <c r="M50" s="1">
-        <v>28.1</v>
+        <v>27.3</v>
       </c>
       <c r="N50" s="1">
-        <v>3.6475245763088601E-3</v>
+        <v>3.2970949919800181E-3</v>
       </c>
       <c r="O50" s="1">
-        <v>2.3130643654641599E-3</v>
+        <v>2.31687756193191E-3</v>
       </c>
       <c r="P50" s="1">
-        <v>1.3724923268537871E-2</v>
+        <v>1.3460167528069861E-2</v>
       </c>
       <c r="Q50" s="1">
-        <v>3.2863529202437611</v>
+        <v>3.237123507396185</v>
       </c>
       <c r="R50" s="1">
-        <v>0.48064810284240023</v>
+        <v>0.44668731063981459</v>
       </c>
       <c r="S50" s="1">
-        <v>62.958639059650331</v>
+        <v>65.029295230351053</v>
       </c>
       <c r="T50" s="1">
-        <v>1.5568702459854949E-3</v>
+        <v>1.559436820531096E-3</v>
       </c>
       <c r="U50" s="1">
-        <v>4.7617988523642192E-2</v>
+        <v>4.7696489039386912E-2</v>
       </c>
       <c r="V50" s="1">
-        <v>38.445424051198778</v>
+        <v>36.327307061575482</v>
       </c>
     </row>
     <row r="51" spans="3:22" x14ac:dyDescent="0.25">
@@ -10523,124 +10550,198 @@
         <v>52</v>
       </c>
       <c r="E51" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F51" s="1">
-        <v>-56.99999999999995</v>
+        <v>-179</v>
       </c>
       <c r="G51" s="1">
-        <v>44933.999999999993</v>
+        <v>44962</v>
       </c>
       <c r="H51" s="1">
-        <v>0.1135665642942983</v>
+        <v>0.1264401049775366</v>
       </c>
       <c r="I51" s="1">
-        <v>20641.733639999999</v>
+        <v>19591.68519</v>
       </c>
       <c r="J51" s="1">
-        <v>0.37868206703164631</v>
+        <v>0.37287042391352693</v>
       </c>
       <c r="K51" s="1">
-        <v>3.4984644144745607E-2</v>
+        <v>3.0603620835372079E-2</v>
       </c>
       <c r="L51" s="1">
-        <v>23.389734217296478</v>
+        <v>22.083162368444469</v>
       </c>
       <c r="M51" s="1">
-        <v>28.8</v>
+        <v>28.1</v>
       </c>
       <c r="N51" s="1">
-        <v>3.7165620688120122E-3</v>
+        <v>3.6475245763088601E-3</v>
       </c>
       <c r="O51" s="1">
-        <v>2.2699959941247069E-3</v>
+        <v>2.3130643654641599E-3</v>
       </c>
       <c r="P51" s="1">
-        <v>1.374237770952952E-2</v>
+        <v>1.3724923268537871E-2</v>
       </c>
       <c r="Q51" s="1">
-        <v>2.790626251836025</v>
+        <v>3.2863529202437611</v>
       </c>
       <c r="R51" s="1">
-        <v>0.49644456313704521</v>
+        <v>0.48064810284240023</v>
       </c>
       <c r="S51" s="1">
-        <v>59.326706022165851</v>
+        <v>62.958639059650331</v>
       </c>
       <c r="T51" s="1">
-        <v>1.491075800062311E-3</v>
+        <v>1.5568702459854949E-3</v>
       </c>
       <c r="U51" s="1">
-        <v>4.775893532736903E-2</v>
+        <v>4.7617988523642192E-2</v>
       </c>
       <c r="V51" s="1">
-        <v>34.524197758490182</v>
+        <v>38.445424051198778</v>
       </c>
     </row>
     <row r="52" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F52" s="1">
+        <v>-56.99999999999995</v>
+      </c>
+      <c r="G52" s="1">
+        <v>44933.999999999993</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.1135665642942983</v>
+      </c>
+      <c r="I52" s="1">
+        <v>20641.733639999999</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.37868206703164631</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3.4984644144745607E-2</v>
+      </c>
+      <c r="L52" s="1">
+        <v>23.389734217296478</v>
+      </c>
+      <c r="M52" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="N52" s="1">
+        <v>3.7165620688120122E-3</v>
+      </c>
+      <c r="O52" s="1">
+        <v>2.2699959941247069E-3</v>
+      </c>
+      <c r="P52" s="1">
+        <v>1.374237770952952E-2</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>2.790626251836025</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0.49644456313704521</v>
+      </c>
+      <c r="S52" s="1">
+        <v>59.326706022165851</v>
+      </c>
+      <c r="T52" s="1">
+        <v>1.491075800062311E-3</v>
+      </c>
+      <c r="U52" s="1">
+        <v>4.775893532736903E-2</v>
+      </c>
+      <c r="V52" s="1">
+        <v>34.524197758490182</v>
+      </c>
+    </row>
+    <row r="53" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="3">
         <v>2020</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F53" s="1">
         <v>-449.99999999999989</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G53" s="1">
         <v>44386</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H53" s="1">
         <v>0.11616275402153831</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I53" s="1">
         <v>21819.183840000002</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J53" s="1">
         <v>0.43312530978236369</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K53" s="1">
         <v>3.4515387734871332E-2</v>
       </c>
-      <c r="L52" s="1">
+      <c r="L53" s="1">
         <v>23.330135132699489</v>
       </c>
-      <c r="M52" s="1">
+      <c r="M53" s="1">
         <v>29.9</v>
       </c>
-      <c r="N52" s="1">
+      <c r="N53" s="1">
         <v>3.807506871536046E-3</v>
       </c>
-      <c r="O52" s="1">
+      <c r="O53" s="1">
         <v>2.343081151714495E-3</v>
       </c>
-      <c r="P52" s="1">
+      <c r="P53" s="1">
         <v>1.4168882079935099E-2</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="Q53" s="1">
         <v>2.863042400756993</v>
       </c>
-      <c r="R52" s="1">
+      <c r="R53" s="1">
         <v>0.49934596494390132</v>
       </c>
-      <c r="S52" s="1">
+      <c r="S53" s="1">
         <v>56.510477592033467</v>
       </c>
-      <c r="T52" s="1">
+      <c r="T53" s="1">
         <v>1.622133105033115E-3</v>
       </c>
-      <c r="U52" s="1">
+      <c r="U53" s="1">
         <v>4.9587707835804067E-2</v>
       </c>
-      <c r="V52" s="1">
+      <c r="V53" s="1">
         <v>33.696300743477607</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I40:I44">
+  <conditionalFormatting sqref="I41:I45">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L41:L45">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -10652,7 +10753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:L44">
+  <conditionalFormatting sqref="Q41:Q45">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -10664,7 +10765,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q40:Q44">
+  <conditionalFormatting sqref="R41:R45">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -10676,7 +10777,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R40:R44">
+  <conditionalFormatting sqref="S41:S45">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -10688,7 +10789,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S40:S44">
+  <conditionalFormatting sqref="V41:V45">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -10700,7 +10801,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V40:V44">
+  <conditionalFormatting sqref="I49:I53">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -10712,7 +10813,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:I52">
+  <conditionalFormatting sqref="L49:L53">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -10724,7 +10825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L48:L52">
+  <conditionalFormatting sqref="Q49:Q53">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -10736,7 +10837,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q48:Q52">
+  <conditionalFormatting sqref="R49:R53">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -10748,7 +10849,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R48:R52">
+  <conditionalFormatting sqref="S49:S53">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -10760,7 +10861,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48:S52">
+  <conditionalFormatting sqref="V49:V53">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -10772,7 +10873,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V48:V52">
+  <conditionalFormatting sqref="G16:T16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -10784,7 +10885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:T15">
+  <conditionalFormatting sqref="G17:T17">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -10796,7 +10897,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:T16">
+  <conditionalFormatting sqref="G18:T18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -10808,7 +10909,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:T17">
+  <conditionalFormatting sqref="G19:T19">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -10820,7 +10921,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18:T18">
+  <conditionalFormatting sqref="G20:T21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -10832,7 +10933,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:T20">
+  <conditionalFormatting sqref="G22:T23">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -10844,7 +10945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:T22">
+  <conditionalFormatting sqref="G24:T25">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -10856,7 +10957,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23:T24">
+  <conditionalFormatting sqref="G26:T27">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -10868,7 +10969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25:T26">
+  <conditionalFormatting sqref="G28:T29">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -10880,7 +10981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27:T28">
+  <conditionalFormatting sqref="G30:T31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>